<commit_message>
Lau - reacomodamiento matriz
</commit_message>
<xml_diff>
--- a/Docs/04-Requerimientos/Proyecto_Final_Status.xlsx
+++ b/Docs/04-Requerimientos/Proyecto_Final_Status.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="118">
   <si>
     <t>COMPLETADO</t>
   </si>
@@ -340,34 +340,55 @@
     <t>25- Conectividad</t>
   </si>
   <si>
-    <t>25.1 Registrar escala de calificaciones.</t>
-  </si>
-  <si>
-    <t>25.2 Registrar Alumnos.</t>
-  </si>
-  <si>
-    <t>25.3 Registrar personal de la institución.</t>
-  </si>
-  <si>
-    <t>25.4 Registrar asignaturas.</t>
-  </si>
-  <si>
-    <t>25.5 Registrar sanciones.</t>
-  </si>
-  <si>
-    <t>25.6 Registrar calificaciones.</t>
-  </si>
-  <si>
-    <t>25.7 Registrar inasistencias de alumnos.</t>
-  </si>
-  <si>
-    <t>25.8 Registrar inasistencias de profesores.</t>
-  </si>
-  <si>
     <t>5.1 Generar reporte de notas de cada una de las materias en los que va del año de un alumno.</t>
   </si>
   <si>
     <t>6.1 Generar reporte estadísticos de desempeño de alumnos en diferentes materias en el período respecto a años anteriores.</t>
+  </si>
+  <si>
+    <t>25.1 Obtener escala de calificaciones.</t>
+  </si>
+  <si>
+    <t>25.2 Obtener Alumnos.</t>
+  </si>
+  <si>
+    <t>25.3 Obtener personal de la institución.</t>
+  </si>
+  <si>
+    <t>25.4 Obtener asignaturas.</t>
+  </si>
+  <si>
+    <t>25.5 Obtener sanciones.</t>
+  </si>
+  <si>
+    <t>25.6 Obtener calificaciones.</t>
+  </si>
+  <si>
+    <t>25.7 Obtener inasistencias de alumnos.</t>
+  </si>
+  <si>
+    <t>25.8 Obtener inasistencias de profesores.</t>
+  </si>
+  <si>
+    <t>21.1 Mantener el sistema disponible en un 97% de lunes a viernes 8 a 18 hs.</t>
+  </si>
+  <si>
+    <t>23.1 Mantener independencia de los motores de bases de datos</t>
+  </si>
+  <si>
+    <t>22.1 Permitir la integración de nuevas funcionalidades.</t>
+  </si>
+  <si>
+    <t>24.1 Registrar administrador de foro.</t>
+  </si>
+  <si>
+    <t>24.2 Modificar administrador de foro.</t>
+  </si>
+  <si>
+    <t>24.3 Eliminar mensaje en foro.</t>
+  </si>
+  <si>
+    <t>1.3 Permitir el logueo del usuario al sistema.</t>
   </si>
 </sst>
 </file>
@@ -1155,8 +1176,8 @@
   <dimension ref="A1:J205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B197" sqref="B197"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1273,9 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -1615,7 +1638,7 @@
         <v>32</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="5"/>
@@ -1693,7 +1716,7 @@
         <v>32</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C37" s="14"/>
       <c r="D37" s="5"/>
@@ -3336,7 +3359,9 @@
     </row>
     <row r="157" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="9"/>
-      <c r="B157" s="9"/>
+      <c r="B157" s="9" t="s">
+        <v>111</v>
+      </c>
       <c r="C157" s="14"/>
       <c r="D157" s="5"/>
       <c r="E157" s="5"/>
@@ -3460,7 +3485,9 @@
     </row>
     <row r="167" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="9"/>
-      <c r="B167" s="9"/>
+      <c r="B167" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="C167" s="14"/>
       <c r="D167" s="5"/>
       <c r="E167" s="5"/>
@@ -3584,7 +3611,9 @@
     </row>
     <row r="177" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="9"/>
-      <c r="B177" s="9"/>
+      <c r="B177" s="9" t="s">
+        <v>112</v>
+      </c>
       <c r="C177" s="14"/>
       <c r="D177" s="5"/>
       <c r="E177" s="5"/>
@@ -3708,7 +3737,9 @@
     </row>
     <row r="187" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A187" s="9"/>
-      <c r="B187" s="9"/>
+      <c r="B187" s="9" t="s">
+        <v>114</v>
+      </c>
       <c r="C187" s="14"/>
       <c r="D187" s="5"/>
       <c r="E187" s="5"/>
@@ -3720,7 +3751,9 @@
     </row>
     <row r="188" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A188" s="9"/>
-      <c r="B188" s="9"/>
+      <c r="B188" s="9" t="s">
+        <v>115</v>
+      </c>
       <c r="C188" s="14"/>
       <c r="D188" s="5"/>
       <c r="E188" s="5"/>
@@ -3732,7 +3765,9 @@
     </row>
     <row r="189" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A189" s="9"/>
-      <c r="B189" s="9"/>
+      <c r="B189" s="9" t="s">
+        <v>116</v>
+      </c>
       <c r="C189" s="14"/>
       <c r="D189" s="5"/>
       <c r="E189" s="5"/>
@@ -3835,7 +3870,7 @@
         <v>59</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C197" s="14"/>
       <c r="D197" s="5"/>
@@ -3851,7 +3886,7 @@
         <v>59</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C198" s="14"/>
       <c r="D198" s="5"/>
@@ -3867,7 +3902,7 @@
         <v>59</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C199" s="14"/>
       <c r="D199" s="5"/>
@@ -3883,7 +3918,7 @@
         <v>59</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C200" s="14"/>
       <c r="D200" s="5"/>
@@ -3899,7 +3934,7 @@
         <v>59</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C201" s="14"/>
       <c r="D201" s="5"/>
@@ -3915,7 +3950,7 @@
         <v>59</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C202" s="14"/>
       <c r="D202" s="5"/>
@@ -3931,7 +3966,7 @@
         <v>59</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C203" s="14"/>
       <c r="D203" s="5"/>
@@ -3947,7 +3982,7 @@
         <v>59</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C204" s="14"/>
       <c r="D204" s="5"/>

</xml_diff>

<commit_message>
Desglose de reportes sobre las encuestas en los niveles docente e institución
</commit_message>
<xml_diff>
--- a/Docs/04-Requerimientos/Proyecto_Final_Status.xlsx
+++ b/Docs/04-Requerimientos/Proyecto_Final_Status.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="132">
   <si>
     <t>COMPLETADO</t>
   </si>
@@ -247,9 +247,6 @@
     <t>8.4 Completar Encuesta</t>
   </si>
   <si>
-    <t xml:space="preserve">9.1 Generar reporte estadístico sobre las encuestas de los alumnos y de los padres. </t>
-  </si>
-  <si>
     <t>Web</t>
   </si>
   <si>
@@ -428,6 +425,12 @@
   </si>
   <si>
     <t>Total Horas Estimadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.1 Generar reporte estadístico sobre las encuestas de docente. </t>
+  </si>
+  <si>
+    <t>9.2 Generar reporte estadístico sobre las encuestas de la institución.</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -634,95 +637,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="51">
     <dxf>
       <fill>
         <patternFill>
@@ -1379,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B198" workbookViewId="0">
-      <selection activeCell="B216" sqref="B216"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1325,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>2</v>
@@ -1414,13 +1334,13 @@
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>2</v>
@@ -1449,7 +1369,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>57</v>
@@ -1468,7 +1388,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>58</v>
@@ -1487,10 +1407,10 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="19">
         <v>18</v>
@@ -1560,7 +1480,7 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>44</v>
@@ -1579,7 +1499,7 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>45</v>
@@ -1807,7 +1727,7 @@
     </row>
     <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>59</v>
@@ -1826,7 +1746,7 @@
     </row>
     <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>60</v>
@@ -1902,7 +1822,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="24">
         <v>20</v>
@@ -1988,7 +1908,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C37" s="25">
         <v>25</v>
@@ -2294,8 +2214,8 @@
       <c r="A56" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B56" s="9" t="s">
-        <v>70</v>
+      <c r="B56" s="29" t="s">
+        <v>130</v>
       </c>
       <c r="C56" s="24">
         <v>25</v>
@@ -2311,7 +2231,9 @@
     </row>
     <row r="57" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
-      <c r="B57" s="9"/>
+      <c r="B57" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="C57" s="24"/>
       <c r="D57" s="14"/>
       <c r="E57" s="5"/>
@@ -3065,7 +2987,7 @@
         <v>9</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C106" s="21"/>
       <c r="D106" s="12"/>
@@ -3082,7 +3004,7 @@
         <v>9</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C107" s="24">
         <v>18</v>
@@ -3101,7 +3023,7 @@
         <v>9</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C108" s="24">
         <v>14</v>
@@ -3120,7 +3042,7 @@
         <v>9</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C109" s="24">
         <v>12</v>
@@ -3215,7 +3137,7 @@
     <row r="116" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C116" s="21"/>
       <c r="D116" s="12"/>
@@ -3232,7 +3154,7 @@
         <v>9</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C117" s="24">
         <v>18</v>
@@ -3353,7 +3275,7 @@
     <row r="126" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C126" s="21"/>
       <c r="D126" s="12"/>
@@ -3370,7 +3292,7 @@
         <v>9</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C127" s="24">
         <v>20</v>
@@ -3389,7 +3311,7 @@
         <v>9</v>
       </c>
       <c r="B128" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C128" s="26">
         <v>26</v>
@@ -3408,7 +3330,7 @@
         <v>9</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C129" s="24">
         <v>26</v>
@@ -3505,7 +3427,7 @@
         <v>24</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C136" s="21"/>
       <c r="D136" s="12"/>
@@ -3522,7 +3444,7 @@
         <v>55</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C137" s="24">
         <v>18</v>
@@ -3541,7 +3463,7 @@
         <v>55</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C138" s="24">
         <v>18</v>
@@ -3560,7 +3482,7 @@
         <v>55</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C139" s="24">
         <v>18</v>
@@ -3579,7 +3501,7 @@
         <v>55</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C140" s="24">
         <v>18</v>
@@ -3598,7 +3520,7 @@
         <v>55</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C141" s="24">
         <v>18</v>
@@ -3669,7 +3591,7 @@
         <v>24</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C146" s="21"/>
       <c r="D146" s="12"/>
@@ -3686,7 +3608,7 @@
         <v>55</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C147" s="24">
         <v>24</v>
@@ -3705,7 +3627,7 @@
         <v>55</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C148" s="24">
         <v>24</v>
@@ -3724,7 +3646,7 @@
         <v>55</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C149" s="24">
         <v>30</v>
@@ -3821,7 +3743,7 @@
         <v>24</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C156" s="21"/>
       <c r="D156" s="12"/>
@@ -3836,7 +3758,7 @@
     <row r="157" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="9"/>
       <c r="B157" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C157" s="24"/>
       <c r="D157" s="14"/>
@@ -3957,7 +3879,7 @@
         <v>24</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C166" s="21"/>
       <c r="D166" s="12"/>
@@ -3972,7 +3894,7 @@
     <row r="167" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="9"/>
       <c r="B167" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C167" s="24"/>
       <c r="D167" s="14"/>
@@ -4093,7 +4015,7 @@
         <v>24</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C176" s="21"/>
       <c r="D176" s="12"/>
@@ -4108,7 +4030,7 @@
     <row r="177" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="9"/>
       <c r="B177" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C177" s="24"/>
       <c r="D177" s="14"/>
@@ -4164,7 +4086,7 @@
         <v>24</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C181" s="21"/>
       <c r="D181" s="12"/>
@@ -4179,7 +4101,7 @@
     <row r="182" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182" s="9"/>
       <c r="B182" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C182" s="24">
         <v>16</v>
@@ -4196,7 +4118,7 @@
     <row r="183" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A183" s="9"/>
       <c r="B183" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C183" s="24">
         <v>16</v>
@@ -4213,7 +4135,7 @@
     <row r="184" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A184" s="9"/>
       <c r="B184" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C184" s="24">
         <v>10</v>
@@ -4284,7 +4206,7 @@
         <v>24</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C189" s="21"/>
       <c r="D189" s="12"/>
@@ -4301,7 +4223,7 @@
         <v>56</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C190" s="24">
         <v>12</v>
@@ -4320,7 +4242,7 @@
         <v>56</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C191" s="24">
         <v>12</v>
@@ -4339,7 +4261,7 @@
         <v>56</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C192" s="24">
         <v>12</v>
@@ -4358,7 +4280,7 @@
         <v>56</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C193" s="24">
         <v>12</v>
@@ -4377,7 +4299,7 @@
         <v>56</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C194" s="24">
         <v>12</v>
@@ -4396,7 +4318,7 @@
         <v>56</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C195" s="24">
         <v>12</v>
@@ -4415,7 +4337,7 @@
         <v>56</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C196" s="24">
         <v>12</v>
@@ -4434,7 +4356,7 @@
         <v>56</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C197" s="24">
         <v>12</v>
@@ -4464,7 +4386,7 @@
     <row r="200" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A200" s="9"/>
       <c r="B200" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C200" s="24"/>
       <c r="D200" s="14"/>
@@ -4479,7 +4401,7 @@
     <row r="201" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="9"/>
       <c r="B201" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C201" s="24">
         <v>40</v>
@@ -4496,7 +4418,7 @@
     <row r="202" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A202" s="9"/>
       <c r="B202" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C202" s="24">
         <v>50</v>
@@ -4513,7 +4435,7 @@
     <row r="203" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="9"/>
       <c r="B203" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C203" s="24">
         <v>50</v>
@@ -4530,7 +4452,7 @@
     <row r="204" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A204" s="9"/>
       <c r="B204" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C204" s="24">
         <v>50</v>
@@ -4547,7 +4469,7 @@
     <row r="205" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205" s="9"/>
       <c r="B205" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C205" s="24">
         <v>80</v>
@@ -4564,7 +4486,7 @@
     <row r="206" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A206" s="9"/>
       <c r="B206" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C206" s="24">
         <v>30</v>
@@ -4581,7 +4503,7 @@
     <row r="207" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207" s="9"/>
       <c r="B207" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C207" s="24">
         <v>100</v>
@@ -4598,7 +4520,7 @@
     <row r="208" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A208" s="9"/>
       <c r="B208" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C208" s="24">
         <v>20</v>
@@ -4615,7 +4537,7 @@
     <row r="209" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="9"/>
       <c r="B209" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C209" s="24">
         <v>50</v>
@@ -4632,7 +4554,7 @@
     <row r="210" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210" s="9"/>
       <c r="B210" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C210" s="24">
         <v>40</v>
@@ -4700,7 +4622,7 @@
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B215" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C215" s="27">
         <f>SUM(C2:C214)</f>
@@ -4709,189 +4631,189 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D8:D45 D72:D99 D48:D55 D57:D69 D200:D204 D176:D188">
-    <cfRule type="containsText" dxfId="62" priority="58" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="50" priority="58" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="59" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="49" priority="59" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="60" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="48" priority="60" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106:D115">
-    <cfRule type="containsText" dxfId="59" priority="55" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="47" priority="55" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D106)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="56" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="46" priority="56" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D106)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="57" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="45" priority="57" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D106)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D116:D125">
-    <cfRule type="containsText" dxfId="56" priority="52" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="44" priority="52" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D116)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="43" priority="53" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D116)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="42" priority="54" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D116)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D126:D135">
-    <cfRule type="containsText" dxfId="53" priority="49" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="41" priority="49" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D126)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="40" priority="50" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D126)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="39" priority="51" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D126)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136:D145">
-    <cfRule type="containsText" dxfId="50" priority="46" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="38" priority="46" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D136)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="37" priority="47" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D136)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="36" priority="48" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D136)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D146:D155">
-    <cfRule type="containsText" dxfId="47" priority="43" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="35" priority="43" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D146)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="44" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D146)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D146)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D156:D165">
-    <cfRule type="containsText" dxfId="44" priority="40" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166:D175">
-    <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="29" priority="37" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D166)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="28" priority="38" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D166)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="27" priority="39" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D166)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D100:D105">
-    <cfRule type="containsText" dxfId="38" priority="25" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="26" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="27" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D100)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70:D71">
-    <cfRule type="containsText" dxfId="35" priority="22" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D70)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="23" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D70)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="24" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189:D198">
-    <cfRule type="containsText" dxfId="32" priority="19" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D189)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="20" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D189)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="21" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D189)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46:D47">
-    <cfRule type="containsText" dxfId="29" priority="16" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="17" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="18" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56">
-    <cfRule type="containsText" dxfId="26" priority="13" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="14" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="15" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D205">
-    <cfRule type="containsText" dxfId="23" priority="10" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D205)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D205)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="12" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D205)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D206">
-    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D206)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D206)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D206)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D207">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D207)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D207)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D208:D214">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="NO COMENZADO">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D208)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D208)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="COMPLETADO">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="COMPLETADO">
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D208)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Se eliminaron los alcances conscernientes a los preceptores a nivel de reportes estratégicos
</commit_message>
<xml_diff>
--- a/Docs/04-Requerimientos/Proyecto_Final_Status.xlsx
+++ b/Docs/04-Requerimientos/Proyecto_Final_Status.xlsx
@@ -24,8 +24,8 @@
     <definedName name="_Toc220775284" localSheetId="0">Sheet1!$B$66</definedName>
     <definedName name="_Toc220775285" localSheetId="0">Sheet1!$B$74</definedName>
     <definedName name="_Toc220775286" localSheetId="0">Sheet1!$B$80</definedName>
-    <definedName name="_Toc220775287" localSheetId="0">Sheet1!$B$90</definedName>
-    <definedName name="_Toc220775288" localSheetId="0">Sheet1!$B$95</definedName>
+    <definedName name="_Toc220775287" localSheetId="0">Sheet1!#REF!</definedName>
+    <definedName name="_Toc220775288" localSheetId="0">Sheet1!$B$86</definedName>
     <definedName name="_Toc220775289" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="_Toc290939942" localSheetId="0">Sheet1!$A$2</definedName>
     <definedName name="_Toc439994688" localSheetId="0">Sheet1!$B$2</definedName>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="131">
   <si>
     <t>COMPLETADO</t>
   </si>
@@ -103,12 +103,6 @@
     <t>13- Generar reportes estratégicos para el gabinete psicopedagógico</t>
   </si>
   <si>
-    <t>14- Generar reportes estratégicos para los preceptores</t>
-  </si>
-  <si>
-    <t>15- Generar reportes estratégicos para la dirección</t>
-  </si>
-  <si>
     <t>Requisitos NO Funcionales</t>
   </si>
   <si>
@@ -118,12 +112,6 @@
     <t>12.1 Consultar tablero de control Docente: Representación gráfica del nivel de calificaciones de alumnos</t>
   </si>
   <si>
-    <t>15.1 Consultar tablero de control Directivo: Representación gráfica del nivel de calificaciones de cursos</t>
-  </si>
-  <si>
-    <t>15.2 Consultar tablero de control Directivo: Representación gráfica del nivel de calificaciones de asignatura</t>
-  </si>
-  <si>
     <t>1- Proveer una página web de la institución</t>
   </si>
   <si>
@@ -133,27 +121,6 @@
     <t>12.2 Generar reporte de rendimiento de alumnos por periodo</t>
   </si>
   <si>
-    <t>15.3 Consultar tablero de control Directivo: Representación gráfica del nivel de inasistencias de cursos (alumnos)</t>
-  </si>
-  <si>
-    <t>15.4 Consultar tablero de control Directivo: Representación gráfica del nivel de inasistencias de cursos (docentes)</t>
-  </si>
-  <si>
-    <t>15.5 Generar reporte de alumnos y de profesores según sus inasistencias.</t>
-  </si>
-  <si>
-    <t>15.6 Generar reporte de rendimientos de profesores por periodo.</t>
-  </si>
-  <si>
-    <t>15.7 Generar reporte de rendimiento por cursos</t>
-  </si>
-  <si>
-    <t>15.8 Generar reporte de rendimiento por asignatura y curso.</t>
-  </si>
-  <si>
-    <t>15.9 Generar reporte estadístico de uso sobre la cantidad de accesos a la autogestión por mes.</t>
-  </si>
-  <si>
     <t>11.1 Generar mensaje.</t>
   </si>
   <si>
@@ -250,129 +217,12 @@
     <t>Web</t>
   </si>
   <si>
-    <t>16- Registrar plan anual de clases</t>
-  </si>
-  <si>
-    <t>17- Registrar temas desarrollados en clases</t>
-  </si>
-  <si>
-    <t>16.1 Registrar planificación de clases</t>
-  </si>
-  <si>
-    <t>16.2 Consultar Planificación</t>
-  </si>
-  <si>
-    <t>16.3 Asignar fecha y hora de contenido</t>
-  </si>
-  <si>
-    <t>17.1 Registrar desarrollo real de clase.</t>
-  </si>
-  <si>
-    <t>18- Gestionar temas desarrollados en clases versus temas planificados</t>
-  </si>
-  <si>
-    <t>18.1 Emitir informe de advertencias sobre el desvío de lo estimado y lo real</t>
-  </si>
-  <si>
-    <t>18.2 Consultar tablero de control Docente: Representación gráfica del desvío de la planificación de clases</t>
-  </si>
-  <si>
-    <t>18.3 Consultar tablero de control Directivo: Representación gráfica del desvío de la planificación de clases por curso</t>
-  </si>
-  <si>
-    <t>19- Seguridad</t>
-  </si>
-  <si>
-    <t>19.1 Registrar Perfiles.</t>
-  </si>
-  <si>
-    <t>19.2 Registrar usuario.</t>
-  </si>
-  <si>
-    <t>19.3 Asignar perfil.</t>
-  </si>
-  <si>
-    <t>19.4 Actualizar usuario.</t>
-  </si>
-  <si>
-    <t>19.5 Registrar email</t>
-  </si>
-  <si>
-    <t>20- Auditoria</t>
-  </si>
-  <si>
-    <t>20.1 Registro de logueo E/S al sistema.</t>
-  </si>
-  <si>
-    <t>20.2 Generar estadística de acceso al sistema.</t>
-  </si>
-  <si>
-    <t>20.3 Generar estadística de utilización de sistema según perfiles.</t>
-  </si>
-  <si>
-    <t>21- Disponibilidad</t>
-  </si>
-  <si>
-    <t>22- Escalabilidad</t>
-  </si>
-  <si>
-    <t>23- Plataforma</t>
-  </si>
-  <si>
-    <t>24- Control de foros de discusión</t>
-  </si>
-  <si>
-    <t>25- Conectividad</t>
-  </si>
-  <si>
     <t>5.1 Generar reporte de notas de cada una de las materias en los que va del año de un alumno.</t>
   </si>
   <si>
     <t>6.1 Generar reporte estadísticos de desempeño de alumnos en diferentes materias en el período respecto a años anteriores.</t>
   </si>
   <si>
-    <t>25.1 Obtener escala de calificaciones.</t>
-  </si>
-  <si>
-    <t>25.2 Obtener Alumnos.</t>
-  </si>
-  <si>
-    <t>25.3 Obtener personal de la institución.</t>
-  </si>
-  <si>
-    <t>25.4 Obtener asignaturas.</t>
-  </si>
-  <si>
-    <t>25.5 Obtener sanciones.</t>
-  </si>
-  <si>
-    <t>25.6 Obtener calificaciones.</t>
-  </si>
-  <si>
-    <t>25.7 Obtener inasistencias de alumnos.</t>
-  </si>
-  <si>
-    <t>25.8 Obtener inasistencias de profesores.</t>
-  </si>
-  <si>
-    <t>21.1 Mantener el sistema disponible en un 97% de lunes a viernes 8 a 18 hs.</t>
-  </si>
-  <si>
-    <t>23.1 Mantener independencia de los motores de bases de datos</t>
-  </si>
-  <si>
-    <t>22.1 Permitir la integración de nuevas funcionalidades.</t>
-  </si>
-  <si>
-    <t>24.1 Registrar administrador de foro.</t>
-  </si>
-  <si>
-    <t>24.2 Modificar administrador de foro.</t>
-  </si>
-  <si>
-    <t>24.3 Eliminar mensaje en foro.</t>
-  </si>
-  <si>
     <t>1.3 Permitir el logueo del usuario al sistema.</t>
   </si>
   <si>
@@ -400,9 +250,6 @@
     <t>4- Desarrollar Plataforma para envio de mensajeria de texto</t>
   </si>
   <si>
-    <t>26- Actividades adicionales</t>
-  </si>
-  <si>
     <t>5- Desarrollar Plataforma para tablero de control</t>
   </si>
   <si>
@@ -431,6 +278,156 @@
   </si>
   <si>
     <t>9.2 Generar reporte estadístico sobre las encuestas de la institución.</t>
+  </si>
+  <si>
+    <t>14- Generar reportes estratégicos para la dirección</t>
+  </si>
+  <si>
+    <t>14.1 Consultar tablero de control Directivo: Representación gráfica del nivel de calificaciones de cursos</t>
+  </si>
+  <si>
+    <t>14.2 Consultar tablero de control Directivo: Representación gráfica del nivel de calificaciones de asignatura</t>
+  </si>
+  <si>
+    <t>14.3 Consultar tablero de control Directivo: Representación gráfica del nivel de inasistencias de cursos (alumnos)</t>
+  </si>
+  <si>
+    <t>14.4 Consultar tablero de control Directivo: Representación gráfica del nivel de inasistencias de cursos (docentes)</t>
+  </si>
+  <si>
+    <t>14.5 Generar reporte de alumnos y de profesores según sus inasistencias.</t>
+  </si>
+  <si>
+    <t>14.6 Generar reporte de rendimientos de profesores por periodo.</t>
+  </si>
+  <si>
+    <t>14.7 Generar reporte de rendimiento por cursos</t>
+  </si>
+  <si>
+    <t>14.8 Generar reporte de rendimiento por asignatura y curso.</t>
+  </si>
+  <si>
+    <t>14.9 Generar reporte estadístico de uso sobre la cantidad de accesos a la autogestión por mes.</t>
+  </si>
+  <si>
+    <t>15- Registrar plan anual de clases</t>
+  </si>
+  <si>
+    <t>15.1 Registrar planificación de clases</t>
+  </si>
+  <si>
+    <t>15.2 Consultar Planificación</t>
+  </si>
+  <si>
+    <t>15.3 Asignar fecha y hora de contenido</t>
+  </si>
+  <si>
+    <t>16- Registrar temas desarrollados en clases</t>
+  </si>
+  <si>
+    <t>16.1 Registrar desarrollo real de clase.</t>
+  </si>
+  <si>
+    <t>17- Gestionar temas desarrollados en clases versus temas planificados</t>
+  </si>
+  <si>
+    <t>17.1 Emitir informe de advertencias sobre el desvío de lo estimado y lo real</t>
+  </si>
+  <si>
+    <t>17.2 Consultar tablero de control Docente: Representación gráfica del desvío de la planificación de clases</t>
+  </si>
+  <si>
+    <t>17.3 Consultar tablero de control Directivo: Representación gráfica del desvío de la planificación de clases por curso</t>
+  </si>
+  <si>
+    <t>18- Seguridad</t>
+  </si>
+  <si>
+    <t>18.1 Registrar Perfiles.</t>
+  </si>
+  <si>
+    <t>18.2 Registrar usuario.</t>
+  </si>
+  <si>
+    <t>18.3 Asignar perfil.</t>
+  </si>
+  <si>
+    <t>18.4 Actualizar usuario.</t>
+  </si>
+  <si>
+    <t>18.5 Registrar email</t>
+  </si>
+  <si>
+    <t>19- Auditoria</t>
+  </si>
+  <si>
+    <t>19.1 Registro de logueo E/S al sistema.</t>
+  </si>
+  <si>
+    <t>19.2 Generar estadística de acceso al sistema.</t>
+  </si>
+  <si>
+    <t>19.3 Generar estadística de utilización de sistema según perfiles.</t>
+  </si>
+  <si>
+    <t>20- Disponibilidad</t>
+  </si>
+  <si>
+    <t>20.1 Mantener el sistema disponible en un 97% de lunes a viernes 8 a 18 hs.</t>
+  </si>
+  <si>
+    <t>21- Escalabilidad</t>
+  </si>
+  <si>
+    <t>21.1 Permitir la integración de nuevas funcionalidades.</t>
+  </si>
+  <si>
+    <t>22- Plataforma</t>
+  </si>
+  <si>
+    <t>22.1 Mantener independencia de los motores de bases de datos</t>
+  </si>
+  <si>
+    <t>23- Control de foros de discusión</t>
+  </si>
+  <si>
+    <t>23.1 Registrar administrador de foro.</t>
+  </si>
+  <si>
+    <t>23.2 Modificar administrador de foro.</t>
+  </si>
+  <si>
+    <t>23.3 Eliminar mensaje en foro.</t>
+  </si>
+  <si>
+    <t>26- Conectividad</t>
+  </si>
+  <si>
+    <t>26.1 Obtener escala de calificaciones.</t>
+  </si>
+  <si>
+    <t>26.2 Obtener Alumnos.</t>
+  </si>
+  <si>
+    <t>26.3 Obtener personal de la institución.</t>
+  </si>
+  <si>
+    <t>26.4 Obtener asignaturas.</t>
+  </si>
+  <si>
+    <t>26.5 Obtener sanciones.</t>
+  </si>
+  <si>
+    <t>26.6 Obtener calificaciones.</t>
+  </si>
+  <si>
+    <t>26.7 Obtener inasistencias de alumnos.</t>
+  </si>
+  <si>
+    <t>26.8 Obtener inasistencias de profesores.</t>
+  </si>
+  <si>
+    <t>27- Actividades adicionales</t>
   </si>
 </sst>
 </file>
@@ -1297,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K215"/>
+  <dimension ref="A1:K206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,7 +1322,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>2</v>
@@ -1334,13 +1331,13 @@
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>2</v>
@@ -1349,13 +1346,13 @@
         <v>6</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="12"/>
@@ -1369,10 +1366,10 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C3" s="19">
         <v>16</v>
@@ -1388,10 +1385,10 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C4" s="19">
         <v>12</v>
@@ -1407,10 +1404,10 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="C5" s="19">
         <v>18</v>
@@ -1480,10 +1477,10 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C10" s="19">
         <v>10</v>
@@ -1499,10 +1496,10 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C11" s="23">
         <v>16</v>
@@ -1572,10 +1569,10 @@
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C16" s="19">
         <v>24</v>
@@ -1591,10 +1588,10 @@
     </row>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C17" s="19">
         <v>18</v>
@@ -1610,10 +1607,10 @@
     </row>
     <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C18" s="19">
         <v>18</v>
@@ -1629,10 +1626,10 @@
     </row>
     <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C19" s="19">
         <v>18</v>
@@ -1648,10 +1645,10 @@
     </row>
     <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C20" s="19">
         <v>18</v>
@@ -1667,10 +1664,10 @@
     </row>
     <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C21" s="19">
         <v>14</v>
@@ -1727,10 +1724,10 @@
     </row>
     <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C25" s="24">
         <v>16</v>
@@ -1746,10 +1743,10 @@
     </row>
     <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C26" s="24">
         <v>12</v>
@@ -1819,10 +1816,10 @@
     </row>
     <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C31" s="24">
         <v>20</v>
@@ -1905,10 +1902,10 @@
     </row>
     <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="C37" s="25">
         <v>25</v>
@@ -1978,10 +1975,10 @@
     </row>
     <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C42" s="24">
         <v>40</v>
@@ -1997,10 +1994,10 @@
     </row>
     <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C43" s="24">
         <v>12</v>
@@ -2016,10 +2013,10 @@
     </row>
     <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C44" s="24">
         <v>20</v>
@@ -2035,10 +2032,10 @@
     </row>
     <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C45" s="24">
         <v>10</v>
@@ -2095,10 +2092,10 @@
     </row>
     <row r="49" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C49" s="24">
         <v>40</v>
@@ -2114,10 +2111,10 @@
     </row>
     <row r="50" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C50" s="24">
         <v>10</v>
@@ -2133,10 +2130,10 @@
     </row>
     <row r="51" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C51" s="24">
         <v>20</v>
@@ -2152,10 +2149,10 @@
     </row>
     <row r="52" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C52" s="24">
         <v>10</v>
@@ -2212,10 +2209,10 @@
     </row>
     <row r="56" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="C56" s="24">
         <v>25</v>
@@ -2232,7 +2229,7 @@
     <row r="57" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="B57" s="9" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="C57" s="24"/>
       <c r="D57" s="14"/>
@@ -2287,10 +2284,10 @@
     </row>
     <row r="61" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C61" s="24">
         <v>20</v>
@@ -2306,10 +2303,10 @@
     </row>
     <row r="62" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C62" s="24">
         <v>20</v>
@@ -2379,10 +2376,10 @@
     </row>
     <row r="67" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C67" s="24">
         <v>12</v>
@@ -2398,10 +2395,10 @@
     </row>
     <row r="68" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C68" s="24">
         <v>15</v>
@@ -2417,10 +2414,10 @@
     </row>
     <row r="69" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C69" s="24">
         <v>10</v>
@@ -2506,7 +2503,7 @@
         <v>9</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C75" s="23">
         <v>15</v>
@@ -2522,10 +2519,10 @@
     </row>
     <row r="76" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C76" s="19">
         <v>22</v>
@@ -2541,10 +2538,10 @@
     </row>
     <row r="77" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C77" s="19">
         <v>22</v>
@@ -2664,23 +2661,31 @@
       <c r="J85" s="5"/>
       <c r="K85" s="5"/>
     </row>
-    <row r="86" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="9"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="24"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="16"/>
-      <c r="F86" s="16"/>
-      <c r="G86" s="16"/>
-      <c r="H86" s="16"/>
-      <c r="I86" s="16"/>
-      <c r="J86" s="16"/>
-      <c r="K86" s="16"/>
+    <row r="86" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+      <c r="B86" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C86" s="21"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
+      <c r="I86" s="10"/>
+      <c r="J86" s="10"/>
+      <c r="K86" s="10"/>
     </row>
     <row r="87" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="9"/>
-      <c r="B87" s="9"/>
-      <c r="C87" s="24"/>
+      <c r="A87" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C87" s="26">
+        <v>12</v>
+      </c>
       <c r="D87" s="14"/>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
@@ -2691,22 +2696,34 @@
       <c r="K87" s="5"/>
     </row>
     <row r="88" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="9"/>
-      <c r="B88" s="9"/>
-      <c r="C88" s="24"/>
+      <c r="A88" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C88" s="24">
+        <v>12</v>
+      </c>
       <c r="D88" s="14"/>
-      <c r="E88" s="16"/>
-      <c r="F88" s="16"/>
-      <c r="G88" s="16"/>
-      <c r="H88" s="16"/>
-      <c r="I88" s="16"/>
-      <c r="J88" s="16"/>
-      <c r="K88" s="16"/>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="22"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+    </row>
+    <row r="89" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C89" s="24">
+        <v>12</v>
+      </c>
       <c r="D89" s="14"/>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
@@ -2716,25 +2733,35 @@
       <c r="J89" s="5"/>
       <c r="K89" s="5"/>
     </row>
-    <row r="90" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C90" s="21"/>
-      <c r="D90" s="12"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="10"/>
-      <c r="H90" s="10"/>
-      <c r="I90" s="10"/>
-      <c r="J90" s="10"/>
-      <c r="K90" s="10"/>
+    <row r="90" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C90" s="24">
+        <v>12</v>
+      </c>
+      <c r="D90" s="14"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
     </row>
     <row r="91" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="9"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="24"/>
+      <c r="A91" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C91" s="24">
+        <v>20</v>
+      </c>
       <c r="D91" s="14"/>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
@@ -2745,9 +2772,15 @@
       <c r="K91" s="5"/>
     </row>
     <row r="92" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="9"/>
-      <c r="B92" s="9"/>
-      <c r="C92" s="24"/>
+      <c r="A92" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C92" s="24">
+        <v>20</v>
+      </c>
       <c r="D92" s="14"/>
       <c r="E92" s="5"/>
       <c r="F92" s="5"/>
@@ -2758,9 +2791,15 @@
       <c r="K92" s="5"/>
     </row>
     <row r="93" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="9"/>
-      <c r="B93" s="9"/>
-      <c r="C93" s="24"/>
+      <c r="A93" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C93" s="24">
+        <v>20</v>
+      </c>
       <c r="D93" s="14"/>
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>
@@ -2770,10 +2809,16 @@
       <c r="J93" s="5"/>
       <c r="K93" s="5"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="22"/>
+    <row r="94" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C94" s="24">
+        <v>20</v>
+      </c>
       <c r="D94" s="14"/>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
@@ -2783,31 +2828,29 @@
       <c r="J94" s="5"/>
       <c r="K94" s="5"/>
     </row>
-    <row r="95" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C95" s="21"/>
-      <c r="D95" s="12"/>
-      <c r="E95" s="10"/>
-      <c r="F95" s="10"/>
-      <c r="G95" s="10"/>
-      <c r="H95" s="10"/>
-      <c r="I95" s="10"/>
-      <c r="J95" s="10"/>
-      <c r="K95" s="10"/>
+    <row r="95" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C95" s="24">
+        <v>20</v>
+      </c>
+      <c r="D95" s="14"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
+      <c r="I95" s="5"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
     </row>
     <row r="96" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B96" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C96" s="26">
-        <v>12</v>
-      </c>
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="24"/>
       <c r="D96" s="14"/>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
@@ -2817,34 +2860,32 @@
       <c r="J96" s="5"/>
       <c r="K96" s="5"/>
     </row>
-    <row r="97" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="9" t="s">
+    <row r="97" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B97" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C97" s="24">
-        <v>12</v>
-      </c>
-      <c r="D97" s="14"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
-      <c r="H97" s="5"/>
-      <c r="I97" s="5"/>
-      <c r="J97" s="5"/>
-      <c r="K97" s="5"/>
+      <c r="B97" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C97" s="21"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="J97" s="10"/>
+      <c r="K97" s="10"/>
     </row>
     <row r="98" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="C98" s="24">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="5"/>
@@ -2860,10 +2901,10 @@
         <v>9</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="C99" s="24">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D99" s="14"/>
       <c r="E99" s="5"/>
@@ -2876,13 +2917,13 @@
     </row>
     <row r="100" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="C100" s="24">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="5"/>
@@ -2894,15 +2935,9 @@
       <c r="K100" s="5"/>
     </row>
     <row r="101" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C101" s="24">
-        <v>20</v>
-      </c>
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="24"/>
       <c r="D101" s="14"/>
       <c r="E101" s="5"/>
       <c r="F101" s="5"/>
@@ -2913,15 +2948,9 @@
       <c r="K101" s="5"/>
     </row>
     <row r="102" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B102" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C102" s="24">
-        <v>20</v>
-      </c>
+      <c r="A102" s="9"/>
+      <c r="B102" s="9"/>
+      <c r="C102" s="24"/>
       <c r="D102" s="14"/>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
@@ -2932,15 +2961,9 @@
       <c r="K102" s="5"/>
     </row>
     <row r="103" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C103" s="24">
-        <v>20</v>
-      </c>
+      <c r="A103" s="9"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="24"/>
       <c r="D103" s="14"/>
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
@@ -2951,15 +2974,9 @@
       <c r="K103" s="5"/>
     </row>
     <row r="104" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B104" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C104" s="24">
-        <v>20</v>
-      </c>
+      <c r="A104" s="9"/>
+      <c r="B104" s="9"/>
+      <c r="C104" s="24"/>
       <c r="D104" s="14"/>
       <c r="E104" s="5"/>
       <c r="F104" s="5"/>
@@ -2982,51 +2999,43 @@
       <c r="J105" s="5"/>
       <c r="K105" s="5"/>
     </row>
-    <row r="106" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C106" s="21"/>
-      <c r="D106" s="12"/>
-      <c r="E106" s="10"/>
-      <c r="F106" s="10"/>
-      <c r="G106" s="10"/>
-      <c r="H106" s="10"/>
-      <c r="I106" s="10"/>
-      <c r="J106" s="10"/>
-      <c r="K106" s="10"/>
-    </row>
-    <row r="107" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B107" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C107" s="24">
-        <v>18</v>
-      </c>
-      <c r="D107" s="14"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="5"/>
-      <c r="G107" s="5"/>
-      <c r="H107" s="5"/>
-      <c r="I107" s="5"/>
-      <c r="J107" s="5"/>
-      <c r="K107" s="5"/>
+    <row r="106" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="9"/>
+      <c r="B106" s="9"/>
+      <c r="C106" s="24"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5"/>
+      <c r="H106" s="5"/>
+      <c r="I106" s="5"/>
+      <c r="J106" s="5"/>
+      <c r="K106" s="5"/>
+    </row>
+    <row r="107" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C107" s="21"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="10"/>
+      <c r="G107" s="10"/>
+      <c r="H107" s="10"/>
+      <c r="I107" s="10"/>
+      <c r="J107" s="10"/>
+      <c r="K107" s="10"/>
     </row>
     <row r="108" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C108" s="24">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="5"/>
@@ -3038,15 +3047,9 @@
       <c r="K108" s="5"/>
     </row>
     <row r="109" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B109" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C109" s="24">
-        <v>12</v>
-      </c>
+      <c r="A109" s="9"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="24"/>
       <c r="D109" s="14"/>
       <c r="E109" s="5"/>
       <c r="F109" s="5"/>
@@ -3134,44 +3137,44 @@
       <c r="J115" s="5"/>
       <c r="K115" s="5"/>
     </row>
-    <row r="116" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A116" s="4"/>
-      <c r="B116" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C116" s="21"/>
-      <c r="D116" s="12"/>
-      <c r="E116" s="10"/>
-      <c r="F116" s="10"/>
-      <c r="G116" s="10"/>
-      <c r="H116" s="10"/>
-      <c r="I116" s="10"/>
-      <c r="J116" s="10"/>
-      <c r="K116" s="10"/>
-    </row>
-    <row r="117" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="9" t="s">
+    <row r="116" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="9"/>
+      <c r="B116" s="9"/>
+      <c r="C116" s="24"/>
+      <c r="D116" s="14"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="5"/>
+      <c r="I116" s="5"/>
+      <c r="J116" s="5"/>
+      <c r="K116" s="5"/>
+    </row>
+    <row r="117" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C117" s="21"/>
+      <c r="D117" s="12"/>
+      <c r="E117" s="10"/>
+      <c r="F117" s="10"/>
+      <c r="G117" s="10"/>
+      <c r="H117" s="10"/>
+      <c r="I117" s="10"/>
+      <c r="J117" s="10"/>
+      <c r="K117" s="10"/>
+    </row>
+    <row r="118" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A118" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B117" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C117" s="24">
-        <v>18</v>
-      </c>
-      <c r="D117" s="14"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
-      <c r="G117" s="5"/>
-      <c r="H117" s="5"/>
-      <c r="I117" s="5"/>
-      <c r="J117" s="5"/>
-      <c r="K117" s="5"/>
-    </row>
-    <row r="118" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A118" s="9"/>
-      <c r="B118" s="9"/>
-      <c r="C118" s="24"/>
+      <c r="B118" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C118" s="24">
+        <v>20</v>
+      </c>
       <c r="D118" s="14"/>
       <c r="E118" s="5"/>
       <c r="F118" s="5"/>
@@ -3182,9 +3185,15 @@
       <c r="K118" s="5"/>
     </row>
     <row r="119" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="9"/>
-      <c r="B119" s="9"/>
-      <c r="C119" s="24"/>
+      <c r="A119" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B119" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C119" s="26">
+        <v>26</v>
+      </c>
       <c r="D119" s="14"/>
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
@@ -3195,9 +3204,15 @@
       <c r="K119" s="5"/>
     </row>
     <row r="120" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="9"/>
-      <c r="B120" s="9"/>
-      <c r="C120" s="24"/>
+      <c r="A120" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C120" s="24">
+        <v>26</v>
+      </c>
       <c r="D120" s="14"/>
       <c r="E120" s="5"/>
       <c r="F120" s="5"/>
@@ -3272,49 +3287,45 @@
       <c r="J125" s="5"/>
       <c r="K125" s="5"/>
     </row>
-    <row r="126" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A126" s="4"/>
-      <c r="B126" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C126" s="21"/>
-      <c r="D126" s="12"/>
-      <c r="E126" s="10"/>
-      <c r="F126" s="10"/>
-      <c r="G126" s="10"/>
-      <c r="H126" s="10"/>
-      <c r="I126" s="10"/>
-      <c r="J126" s="10"/>
-      <c r="K126" s="10"/>
-    </row>
-    <row r="127" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A127" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B127" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C127" s="24">
-        <v>20</v>
-      </c>
-      <c r="D127" s="14"/>
-      <c r="E127" s="5"/>
-      <c r="F127" s="5"/>
-      <c r="G127" s="5"/>
-      <c r="H127" s="5"/>
-      <c r="I127" s="5"/>
-      <c r="J127" s="5"/>
-      <c r="K127" s="5"/>
+    <row r="126" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A126" s="9"/>
+      <c r="B126" s="9"/>
+      <c r="C126" s="24"/>
+      <c r="D126" s="14"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5"/>
+      <c r="G126" s="5"/>
+      <c r="H126" s="5"/>
+      <c r="I126" s="5"/>
+      <c r="J126" s="5"/>
+      <c r="K126" s="5"/>
+    </row>
+    <row r="127" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C127" s="21"/>
+      <c r="D127" s="12"/>
+      <c r="E127" s="10"/>
+      <c r="F127" s="10"/>
+      <c r="G127" s="10"/>
+      <c r="H127" s="10"/>
+      <c r="I127" s="10"/>
+      <c r="J127" s="10"/>
+      <c r="K127" s="10"/>
     </row>
     <row r="128" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B128" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C128" s="26">
-        <v>26</v>
+        <v>44</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C128" s="24">
+        <v>18</v>
       </c>
       <c r="D128" s="14"/>
       <c r="E128" s="5"/>
@@ -3327,13 +3338,13 @@
     </row>
     <row r="129" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="C129" s="24">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D129" s="14"/>
       <c r="E129" s="5"/>
@@ -3345,9 +3356,15 @@
       <c r="K129" s="5"/>
     </row>
     <row r="130" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A130" s="9"/>
-      <c r="B130" s="9"/>
-      <c r="C130" s="24"/>
+      <c r="A130" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C130" s="24">
+        <v>18</v>
+      </c>
       <c r="D130" s="14"/>
       <c r="E130" s="5"/>
       <c r="F130" s="5"/>
@@ -3358,9 +3375,15 @@
       <c r="K130" s="5"/>
     </row>
     <row r="131" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A131" s="9"/>
-      <c r="B131" s="9"/>
-      <c r="C131" s="24"/>
+      <c r="A131" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C131" s="24">
+        <v>18</v>
+      </c>
       <c r="D131" s="14"/>
       <c r="E131" s="5"/>
       <c r="F131" s="5"/>
@@ -3371,9 +3394,15 @@
       <c r="K131" s="5"/>
     </row>
     <row r="132" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A132" s="9"/>
-      <c r="B132" s="9"/>
-      <c r="C132" s="24"/>
+      <c r="A132" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C132" s="24">
+        <v>18</v>
+      </c>
       <c r="D132" s="14"/>
       <c r="E132" s="5"/>
       <c r="F132" s="5"/>
@@ -3422,51 +3451,45 @@
       <c r="J135" s="5"/>
       <c r="K135" s="5"/>
     </row>
-    <row r="136" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A136" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C136" s="21"/>
-      <c r="D136" s="12"/>
-      <c r="E136" s="10"/>
-      <c r="F136" s="10"/>
-      <c r="G136" s="10"/>
-      <c r="H136" s="10"/>
-      <c r="I136" s="10"/>
-      <c r="J136" s="10"/>
-      <c r="K136" s="10"/>
-    </row>
-    <row r="137" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A137" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B137" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C137" s="24">
-        <v>18</v>
-      </c>
-      <c r="D137" s="14"/>
-      <c r="E137" s="5"/>
-      <c r="F137" s="5"/>
-      <c r="G137" s="5"/>
-      <c r="H137" s="5"/>
-      <c r="I137" s="5"/>
-      <c r="J137" s="5"/>
-      <c r="K137" s="5"/>
+    <row r="136" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A136" s="9"/>
+      <c r="B136" s="9"/>
+      <c r="C136" s="24"/>
+      <c r="D136" s="14"/>
+      <c r="E136" s="5"/>
+      <c r="F136" s="5"/>
+      <c r="G136" s="5"/>
+      <c r="H136" s="5"/>
+      <c r="I136" s="5"/>
+      <c r="J136" s="5"/>
+      <c r="K136" s="5"/>
+    </row>
+    <row r="137" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C137" s="21"/>
+      <c r="D137" s="12"/>
+      <c r="E137" s="10"/>
+      <c r="F137" s="10"/>
+      <c r="G137" s="10"/>
+      <c r="H137" s="10"/>
+      <c r="I137" s="10"/>
+      <c r="J137" s="10"/>
+      <c r="K137" s="10"/>
     </row>
     <row r="138" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C138" s="24">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D138" s="14"/>
       <c r="E138" s="5"/>
@@ -3479,13 +3502,13 @@
     </row>
     <row r="139" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="9" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="C139" s="24">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D139" s="14"/>
       <c r="E139" s="5"/>
@@ -3498,13 +3521,13 @@
     </row>
     <row r="140" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="C140" s="24">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D140" s="14"/>
       <c r="E140" s="5"/>
@@ -3516,15 +3539,9 @@
       <c r="K140" s="5"/>
     </row>
     <row r="141" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A141" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B141" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C141" s="24">
-        <v>18</v>
-      </c>
+      <c r="A141" s="9"/>
+      <c r="B141" s="9"/>
+      <c r="C141" s="24"/>
       <c r="D141" s="14"/>
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
@@ -3586,52 +3603,42 @@
       <c r="J145" s="5"/>
       <c r="K145" s="5"/>
     </row>
-    <row r="146" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A146" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B146" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C146" s="21"/>
-      <c r="D146" s="12"/>
-      <c r="E146" s="10"/>
-      <c r="F146" s="10"/>
-      <c r="G146" s="10"/>
-      <c r="H146" s="10"/>
-      <c r="I146" s="10"/>
-      <c r="J146" s="10"/>
-      <c r="K146" s="10"/>
-    </row>
-    <row r="147" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A147" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B147" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C147" s="24">
-        <v>24</v>
-      </c>
-      <c r="D147" s="14"/>
-      <c r="E147" s="5"/>
-      <c r="F147" s="5"/>
-      <c r="G147" s="5"/>
-      <c r="H147" s="5"/>
-      <c r="I147" s="5"/>
-      <c r="J147" s="5"/>
-      <c r="K147" s="5"/>
+    <row r="146" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A146" s="9"/>
+      <c r="B146" s="9"/>
+      <c r="C146" s="24"/>
+      <c r="D146" s="14"/>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5"/>
+      <c r="G146" s="5"/>
+      <c r="H146" s="5"/>
+      <c r="I146" s="5"/>
+      <c r="J146" s="5"/>
+      <c r="K146" s="5"/>
+    </row>
+    <row r="147" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C147" s="21"/>
+      <c r="D147" s="12"/>
+      <c r="E147" s="10"/>
+      <c r="F147" s="10"/>
+      <c r="G147" s="10"/>
+      <c r="H147" s="10"/>
+      <c r="I147" s="10"/>
+      <c r="J147" s="10"/>
+      <c r="K147" s="10"/>
     </row>
     <row r="148" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A148" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="A148" s="9"/>
       <c r="B148" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C148" s="24">
-        <v>24</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="C148" s="24"/>
       <c r="D148" s="14"/>
       <c r="E148" s="5"/>
       <c r="F148" s="5"/>
@@ -3642,15 +3649,9 @@
       <c r="K148" s="5"/>
     </row>
     <row r="149" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A149" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B149" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C149" s="24">
-        <v>30</v>
-      </c>
+      <c r="A149" s="9"/>
+      <c r="B149" s="9"/>
+      <c r="C149" s="24"/>
       <c r="D149" s="14"/>
       <c r="E149" s="5"/>
       <c r="F149" s="5"/>
@@ -3738,41 +3739,41 @@
       <c r="J155" s="5"/>
       <c r="K155" s="5"/>
     </row>
-    <row r="156" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A156" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B156" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C156" s="21"/>
-      <c r="D156" s="12"/>
-      <c r="E156" s="10"/>
-      <c r="F156" s="10"/>
-      <c r="G156" s="10"/>
-      <c r="H156" s="10"/>
-      <c r="I156" s="10"/>
-      <c r="J156" s="10"/>
-      <c r="K156" s="10"/>
-    </row>
-    <row r="157" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A157" s="9"/>
-      <c r="B157" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C157" s="24"/>
-      <c r="D157" s="14"/>
-      <c r="E157" s="5"/>
-      <c r="F157" s="5"/>
-      <c r="G157" s="5"/>
-      <c r="H157" s="5"/>
-      <c r="I157" s="5"/>
-      <c r="J157" s="5"/>
-      <c r="K157" s="5"/>
+    <row r="156" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A156" s="9"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="24"/>
+      <c r="D156" s="14"/>
+      <c r="E156" s="5"/>
+      <c r="F156" s="5"/>
+      <c r="G156" s="5"/>
+      <c r="H156" s="5"/>
+      <c r="I156" s="5"/>
+      <c r="J156" s="5"/>
+      <c r="K156" s="5"/>
+    </row>
+    <row r="157" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A157" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C157" s="21"/>
+      <c r="D157" s="12"/>
+      <c r="E157" s="10"/>
+      <c r="F157" s="10"/>
+      <c r="G157" s="10"/>
+      <c r="H157" s="10"/>
+      <c r="I157" s="10"/>
+      <c r="J157" s="10"/>
+      <c r="K157" s="10"/>
     </row>
     <row r="158" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="9"/>
-      <c r="B158" s="9"/>
+      <c r="B158" s="9" t="s">
+        <v>114</v>
+      </c>
       <c r="C158" s="24"/>
       <c r="D158" s="14"/>
       <c r="E158" s="5"/>
@@ -3874,41 +3875,41 @@
       <c r="J165" s="5"/>
       <c r="K165" s="5"/>
     </row>
-    <row r="166" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A166" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B166" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C166" s="21"/>
-      <c r="D166" s="12"/>
-      <c r="E166" s="10"/>
-      <c r="F166" s="10"/>
-      <c r="G166" s="10"/>
-      <c r="H166" s="10"/>
-      <c r="I166" s="10"/>
-      <c r="J166" s="10"/>
-      <c r="K166" s="10"/>
-    </row>
-    <row r="167" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A167" s="9"/>
-      <c r="B167" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C167" s="24"/>
-      <c r="D167" s="14"/>
-      <c r="E167" s="5"/>
-      <c r="F167" s="5"/>
-      <c r="G167" s="5"/>
-      <c r="H167" s="5"/>
-      <c r="I167" s="5"/>
-      <c r="J167" s="5"/>
-      <c r="K167" s="5"/>
+    <row r="166" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A166" s="9"/>
+      <c r="B166" s="9"/>
+      <c r="C166" s="24"/>
+      <c r="D166" s="14"/>
+      <c r="E166" s="5"/>
+      <c r="F166" s="5"/>
+      <c r="G166" s="5"/>
+      <c r="H166" s="5"/>
+      <c r="I166" s="5"/>
+      <c r="J166" s="5"/>
+      <c r="K166" s="5"/>
+    </row>
+    <row r="167" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A167" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C167" s="21"/>
+      <c r="D167" s="12"/>
+      <c r="E167" s="10"/>
+      <c r="F167" s="10"/>
+      <c r="G167" s="10"/>
+      <c r="H167" s="10"/>
+      <c r="I167" s="10"/>
+      <c r="J167" s="10"/>
+      <c r="K167" s="10"/>
     </row>
     <row r="168" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="9"/>
-      <c r="B168" s="9"/>
+      <c r="B168" s="9" t="s">
+        <v>116</v>
+      </c>
       <c r="C168" s="24"/>
       <c r="D168" s="14"/>
       <c r="E168" s="5"/>
@@ -3958,23 +3959,31 @@
       <c r="J171" s="5"/>
       <c r="K171" s="5"/>
     </row>
-    <row r="172" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A172" s="9"/>
-      <c r="B172" s="9"/>
-      <c r="C172" s="24"/>
-      <c r="D172" s="14"/>
-      <c r="E172" s="5"/>
-      <c r="F172" s="5"/>
-      <c r="G172" s="5"/>
-      <c r="H172" s="5"/>
-      <c r="I172" s="5"/>
-      <c r="J172" s="5"/>
-      <c r="K172" s="5"/>
+    <row r="172" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A172" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C172" s="21"/>
+      <c r="D172" s="12"/>
+      <c r="E172" s="10"/>
+      <c r="F172" s="10"/>
+      <c r="G172" s="10"/>
+      <c r="H172" s="10"/>
+      <c r="I172" s="10"/>
+      <c r="J172" s="10"/>
+      <c r="K172" s="10"/>
     </row>
     <row r="173" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="9"/>
-      <c r="B173" s="9"/>
-      <c r="C173" s="24"/>
+      <c r="B173" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C173" s="24">
+        <v>16</v>
+      </c>
       <c r="D173" s="14"/>
       <c r="E173" s="5"/>
       <c r="F173" s="5"/>
@@ -3986,8 +3995,12 @@
     </row>
     <row r="174" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="9"/>
-      <c r="B174" s="9"/>
-      <c r="C174" s="24"/>
+      <c r="B174" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C174" s="24">
+        <v>16</v>
+      </c>
       <c r="D174" s="14"/>
       <c r="E174" s="5"/>
       <c r="F174" s="5"/>
@@ -3999,8 +4012,12 @@
     </row>
     <row r="175" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="9"/>
-      <c r="B175" s="9"/>
-      <c r="C175" s="24"/>
+      <c r="B175" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C175" s="24">
+        <v>10</v>
+      </c>
       <c r="D175" s="14"/>
       <c r="E175" s="5"/>
       <c r="F175" s="5"/>
@@ -4010,28 +4027,22 @@
       <c r="J175" s="5"/>
       <c r="K175" s="5"/>
     </row>
-    <row r="176" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A176" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B176" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C176" s="21"/>
-      <c r="D176" s="12"/>
-      <c r="E176" s="10"/>
-      <c r="F176" s="10"/>
-      <c r="G176" s="10"/>
-      <c r="H176" s="10"/>
-      <c r="I176" s="10"/>
-      <c r="J176" s="10"/>
-      <c r="K176" s="10"/>
+    <row r="176" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A176" s="9"/>
+      <c r="B176" s="9"/>
+      <c r="C176" s="24"/>
+      <c r="D176" s="14"/>
+      <c r="E176" s="5"/>
+      <c r="F176" s="5"/>
+      <c r="G176" s="5"/>
+      <c r="H176" s="5"/>
+      <c r="I176" s="5"/>
+      <c r="J176" s="5"/>
+      <c r="K176" s="5"/>
     </row>
     <row r="177" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="9"/>
-      <c r="B177" s="9" t="s">
-        <v>107</v>
-      </c>
+      <c r="B177" s="9"/>
       <c r="C177" s="24"/>
       <c r="D177" s="14"/>
       <c r="E177" s="5"/>
@@ -4068,43 +4079,51 @@
       <c r="J179" s="5"/>
       <c r="K179" s="5"/>
     </row>
-    <row r="180" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A180" s="9"/>
-      <c r="B180" s="9"/>
-      <c r="C180" s="24"/>
-      <c r="D180" s="14"/>
-      <c r="E180" s="5"/>
-      <c r="F180" s="5"/>
-      <c r="G180" s="5"/>
-      <c r="H180" s="5"/>
-      <c r="I180" s="5"/>
-      <c r="J180" s="5"/>
-      <c r="K180" s="5"/>
-    </row>
-    <row r="181" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A181" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B181" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C181" s="21"/>
-      <c r="D181" s="12"/>
-      <c r="E181" s="10"/>
-      <c r="F181" s="10"/>
-      <c r="G181" s="10"/>
-      <c r="H181" s="10"/>
-      <c r="I181" s="10"/>
-      <c r="J181" s="10"/>
-      <c r="K181" s="10"/>
+    <row r="180" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A180" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C180" s="21"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="10"/>
+      <c r="F180" s="10"/>
+      <c r="G180" s="10"/>
+      <c r="H180" s="10"/>
+      <c r="I180" s="10"/>
+      <c r="J180" s="10"/>
+      <c r="K180" s="10"/>
+    </row>
+    <row r="181" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A181" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B181" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C181" s="24">
+        <v>12</v>
+      </c>
+      <c r="D181" s="14"/>
+      <c r="E181" s="5"/>
+      <c r="F181" s="5"/>
+      <c r="G181" s="5"/>
+      <c r="H181" s="5"/>
+      <c r="I181" s="5"/>
+      <c r="J181" s="5"/>
+      <c r="K181" s="5"/>
     </row>
     <row r="182" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A182" s="9"/>
+      <c r="A182" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="B182" s="9" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="C182" s="24">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D182" s="14"/>
       <c r="E182" s="5"/>
@@ -4116,12 +4135,14 @@
       <c r="K182" s="5"/>
     </row>
     <row r="183" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A183" s="9"/>
+      <c r="A183" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="B183" s="9" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="C183" s="24">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D183" s="14"/>
       <c r="E183" s="5"/>
@@ -4133,12 +4154,14 @@
       <c r="K183" s="5"/>
     </row>
     <row r="184" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A184" s="9"/>
+      <c r="A184" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="B184" s="9" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="C184" s="24">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D184" s="14"/>
       <c r="E184" s="5"/>
@@ -4150,9 +4173,15 @@
       <c r="K184" s="5"/>
     </row>
     <row r="185" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A185" s="9"/>
-      <c r="B185" s="9"/>
-      <c r="C185" s="24"/>
+      <c r="A185" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B185" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C185" s="24">
+        <v>12</v>
+      </c>
       <c r="D185" s="14"/>
       <c r="E185" s="5"/>
       <c r="F185" s="5"/>
@@ -4163,9 +4192,15 @@
       <c r="K185" s="5"/>
     </row>
     <row r="186" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="9"/>
-      <c r="B186" s="9"/>
-      <c r="C186" s="24"/>
+      <c r="A186" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B186" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C186" s="24">
+        <v>12</v>
+      </c>
       <c r="D186" s="14"/>
       <c r="E186" s="5"/>
       <c r="F186" s="5"/>
@@ -4176,9 +4211,15 @@
       <c r="K186" s="5"/>
     </row>
     <row r="187" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A187" s="9"/>
-      <c r="B187" s="9"/>
-      <c r="C187" s="24"/>
+      <c r="A187" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B187" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C187" s="24">
+        <v>12</v>
+      </c>
       <c r="D187" s="14"/>
       <c r="E187" s="5"/>
       <c r="F187" s="5"/>
@@ -4189,9 +4230,15 @@
       <c r="K187" s="5"/>
     </row>
     <row r="188" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A188" s="9"/>
-      <c r="B188" s="9"/>
-      <c r="C188" s="24"/>
+      <c r="A188" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B188" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C188" s="24">
+        <v>12</v>
+      </c>
       <c r="D188" s="14"/>
       <c r="E188" s="5"/>
       <c r="F188" s="5"/>
@@ -4201,52 +4248,25 @@
       <c r="J188" s="5"/>
       <c r="K188" s="5"/>
     </row>
-    <row r="189" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A189" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B189" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C189" s="21"/>
-      <c r="D189" s="12"/>
-      <c r="E189" s="10"/>
-      <c r="F189" s="10"/>
-      <c r="G189" s="10"/>
-      <c r="H189" s="10"/>
-      <c r="I189" s="10"/>
-      <c r="J189" s="10"/>
-      <c r="K189" s="10"/>
-    </row>
-    <row r="190" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A190" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B190" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C190" s="24">
-        <v>12</v>
-      </c>
-      <c r="D190" s="14"/>
-      <c r="E190" s="5"/>
-      <c r="F190" s="5"/>
-      <c r="G190" s="5"/>
-      <c r="H190" s="5"/>
-      <c r="I190" s="5"/>
-      <c r="J190" s="5"/>
-      <c r="K190" s="5"/>
-    </row>
-    <row r="191" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A191" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B191" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C191" s="24">
-        <v>12</v>
-      </c>
+    <row r="189" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A189" s="9"/>
+      <c r="B189" s="9"/>
+      <c r="C189" s="24"/>
+      <c r="D189" s="14"/>
+      <c r="E189" s="5"/>
+      <c r="F189" s="5"/>
+      <c r="G189" s="5"/>
+      <c r="H189" s="5"/>
+      <c r="I189" s="5"/>
+      <c r="J189" s="5"/>
+      <c r="K189" s="5"/>
+    </row>
+    <row r="191" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A191" s="9"/>
+      <c r="B191" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C191" s="24"/>
       <c r="D191" s="14"/>
       <c r="E191" s="5"/>
       <c r="F191" s="5"/>
@@ -4257,14 +4277,12 @@
       <c r="K191" s="5"/>
     </row>
     <row r="192" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A192" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="A192" s="9"/>
       <c r="B192" s="9" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="C192" s="24">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D192" s="14"/>
       <c r="E192" s="5"/>
@@ -4276,14 +4294,12 @@
       <c r="K192" s="5"/>
     </row>
     <row r="193" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A193" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="A193" s="9"/>
       <c r="B193" s="9" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="C193" s="24">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D193" s="14"/>
       <c r="E193" s="5"/>
@@ -4295,14 +4311,12 @@
       <c r="K193" s="5"/>
     </row>
     <row r="194" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A194" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="A194" s="9"/>
       <c r="B194" s="9" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="C194" s="24">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D194" s="14"/>
       <c r="E194" s="5"/>
@@ -4314,14 +4328,12 @@
       <c r="K194" s="5"/>
     </row>
     <row r="195" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A195" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="A195" s="9"/>
       <c r="B195" s="9" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="C195" s="24">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D195" s="14"/>
       <c r="E195" s="5"/>
@@ -4333,14 +4345,12 @@
       <c r="K195" s="5"/>
     </row>
     <row r="196" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A196" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="A196" s="9"/>
       <c r="B196" s="9" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="C196" s="24">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="D196" s="14"/>
       <c r="E196" s="5"/>
@@ -4352,14 +4362,12 @@
       <c r="K196" s="5"/>
     </row>
     <row r="197" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A197" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="A197" s="9"/>
       <c r="B197" s="9" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="C197" s="24">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D197" s="14"/>
       <c r="E197" s="5"/>
@@ -4372,8 +4380,12 @@
     </row>
     <row r="198" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A198" s="9"/>
-      <c r="B198" s="9"/>
-      <c r="C198" s="24"/>
+      <c r="B198" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C198" s="24">
+        <v>100</v>
+      </c>
       <c r="D198" s="14"/>
       <c r="E198" s="5"/>
       <c r="F198" s="5"/>
@@ -4383,12 +4395,31 @@
       <c r="J198" s="5"/>
       <c r="K198" s="5"/>
     </row>
-    <row r="200" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A199" s="9"/>
+      <c r="B199" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C199" s="24">
+        <v>20</v>
+      </c>
+      <c r="D199" s="14"/>
+      <c r="E199" s="5"/>
+      <c r="F199" s="5"/>
+      <c r="G199" s="5"/>
+      <c r="H199" s="5"/>
+      <c r="I199" s="5"/>
+      <c r="J199" s="5"/>
+      <c r="K199" s="5"/>
+    </row>
+    <row r="200" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A200" s="9"/>
-      <c r="B200" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C200" s="24"/>
+      <c r="B200" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C200" s="24">
+        <v>50</v>
+      </c>
       <c r="D200" s="14"/>
       <c r="E200" s="5"/>
       <c r="F200" s="5"/>
@@ -4401,7 +4432,7 @@
     <row r="201" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="9"/>
       <c r="B201" s="9" t="s">
-        <v>128</v>
+        <v>76</v>
       </c>
       <c r="C201" s="24">
         <v>40</v>
@@ -4417,12 +4448,8 @@
     </row>
     <row r="202" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A202" s="9"/>
-      <c r="B202" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C202" s="24">
-        <v>50</v>
-      </c>
+      <c r="B202" s="9"/>
+      <c r="C202" s="24"/>
       <c r="D202" s="14"/>
       <c r="E202" s="5"/>
       <c r="F202" s="5"/>
@@ -4434,12 +4461,8 @@
     </row>
     <row r="203" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="9"/>
-      <c r="B203" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C203" s="24">
-        <v>50</v>
-      </c>
+      <c r="B203" s="9"/>
+      <c r="C203" s="24"/>
       <c r="D203" s="14"/>
       <c r="E203" s="5"/>
       <c r="F203" s="5"/>
@@ -4451,12 +4474,8 @@
     </row>
     <row r="204" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A204" s="9"/>
-      <c r="B204" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C204" s="24">
-        <v>50</v>
-      </c>
+      <c r="B204" s="9"/>
+      <c r="C204" s="24"/>
       <c r="D204" s="14"/>
       <c r="E204" s="5"/>
       <c r="F204" s="5"/>
@@ -4468,12 +4487,8 @@
     </row>
     <row r="205" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205" s="9"/>
-      <c r="B205" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C205" s="24">
-        <v>80</v>
-      </c>
+      <c r="B205" s="9"/>
+      <c r="C205" s="24"/>
       <c r="D205" s="14"/>
       <c r="E205" s="5"/>
       <c r="F205" s="5"/>
@@ -4483,154 +4498,17 @@
       <c r="J205" s="5"/>
       <c r="K205" s="5"/>
     </row>
-    <row r="206" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A206" s="9"/>
-      <c r="B206" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C206" s="24">
-        <v>30</v>
-      </c>
-      <c r="D206" s="14"/>
-      <c r="E206" s="5"/>
-      <c r="F206" s="5"/>
-      <c r="G206" s="5"/>
-      <c r="H206" s="5"/>
-      <c r="I206" s="5"/>
-      <c r="J206" s="5"/>
-      <c r="K206" s="5"/>
-    </row>
-    <row r="207" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A207" s="9"/>
-      <c r="B207" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C207" s="24">
-        <v>100</v>
-      </c>
-      <c r="D207" s="14"/>
-      <c r="E207" s="5"/>
-      <c r="F207" s="5"/>
-      <c r="G207" s="5"/>
-      <c r="H207" s="5"/>
-      <c r="I207" s="5"/>
-      <c r="J207" s="5"/>
-      <c r="K207" s="5"/>
-    </row>
-    <row r="208" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A208" s="9"/>
-      <c r="B208" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C208" s="24">
-        <v>20</v>
-      </c>
-      <c r="D208" s="14"/>
-      <c r="E208" s="5"/>
-      <c r="F208" s="5"/>
-      <c r="G208" s="5"/>
-      <c r="H208" s="5"/>
-      <c r="I208" s="5"/>
-      <c r="J208" s="5"/>
-      <c r="K208" s="5"/>
-    </row>
-    <row r="209" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A209" s="9"/>
-      <c r="B209" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C209" s="24">
-        <v>50</v>
-      </c>
-      <c r="D209" s="14"/>
-      <c r="E209" s="5"/>
-      <c r="F209" s="5"/>
-      <c r="G209" s="5"/>
-      <c r="H209" s="5"/>
-      <c r="I209" s="5"/>
-      <c r="J209" s="5"/>
-      <c r="K209" s="5"/>
-    </row>
-    <row r="210" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A210" s="9"/>
-      <c r="B210" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C210" s="24">
-        <v>40</v>
-      </c>
-      <c r="D210" s="14"/>
-      <c r="E210" s="5"/>
-      <c r="F210" s="5"/>
-      <c r="G210" s="5"/>
-      <c r="H210" s="5"/>
-      <c r="I210" s="5"/>
-      <c r="J210" s="5"/>
-      <c r="K210" s="5"/>
-    </row>
-    <row r="211" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A211" s="9"/>
-      <c r="B211" s="9"/>
-      <c r="C211" s="24"/>
-      <c r="D211" s="14"/>
-      <c r="E211" s="5"/>
-      <c r="F211" s="5"/>
-      <c r="G211" s="5"/>
-      <c r="H211" s="5"/>
-      <c r="I211" s="5"/>
-      <c r="J211" s="5"/>
-      <c r="K211" s="5"/>
-    </row>
-    <row r="212" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A212" s="9"/>
-      <c r="B212" s="9"/>
-      <c r="C212" s="24"/>
-      <c r="D212" s="14"/>
-      <c r="E212" s="5"/>
-      <c r="F212" s="5"/>
-      <c r="G212" s="5"/>
-      <c r="H212" s="5"/>
-      <c r="I212" s="5"/>
-      <c r="J212" s="5"/>
-      <c r="K212" s="5"/>
-    </row>
-    <row r="213" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A213" s="9"/>
-      <c r="B213" s="9"/>
-      <c r="C213" s="24"/>
-      <c r="D213" s="14"/>
-      <c r="E213" s="5"/>
-      <c r="F213" s="5"/>
-      <c r="G213" s="5"/>
-      <c r="H213" s="5"/>
-      <c r="I213" s="5"/>
-      <c r="J213" s="5"/>
-      <c r="K213" s="5"/>
-    </row>
-    <row r="214" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A214" s="9"/>
-      <c r="B214" s="9"/>
-      <c r="C214" s="24"/>
-      <c r="D214" s="14"/>
-      <c r="E214" s="5"/>
-      <c r="F214" s="5"/>
-      <c r="G214" s="5"/>
-      <c r="H214" s="5"/>
-      <c r="I214" s="5"/>
-      <c r="J214" s="5"/>
-      <c r="K214" s="5"/>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B215" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="C215" s="27">
-        <f>SUM(C2:C214)</f>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B206" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C206" s="27">
+        <f>SUM(C2:C205)</f>
         <v>1676</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D8:D45 D72:D99 D48:D55 D57:D69 D200:D204 D176:D188">
+  <conditionalFormatting sqref="D8:D45 D48:D55 D57:D69 D191:D195 D167:D179 D72:D90">
     <cfRule type="containsText" dxfId="50" priority="58" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D8)))</formula>
     </cfRule>
@@ -4641,92 +4519,92 @@
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D106:D115">
+  <conditionalFormatting sqref="D97:D106">
     <cfRule type="containsText" dxfId="47" priority="55" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D97)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="46" priority="56" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D97)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="45" priority="57" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D97)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D116:D125">
+  <conditionalFormatting sqref="D107:D116">
     <cfRule type="containsText" dxfId="44" priority="52" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D116)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="43" priority="53" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D116)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="42" priority="54" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D116)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D107)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D126:D135">
+  <conditionalFormatting sqref="D117:D126">
     <cfRule type="containsText" dxfId="41" priority="49" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D126)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D117)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="40" priority="50" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D126)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D117)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="39" priority="51" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D126)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D117)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D136:D145">
+  <conditionalFormatting sqref="D127:D136">
     <cfRule type="containsText" dxfId="38" priority="46" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D136)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D127)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="37" priority="47" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D136)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D127)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="36" priority="48" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D136)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D127)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D146:D155">
+  <conditionalFormatting sqref="D137:D146">
     <cfRule type="containsText" dxfId="35" priority="43" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D146)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D137)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D146)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D137)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D146)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D137)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D156:D165">
+  <conditionalFormatting sqref="D147:D156">
     <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D156)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D147)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D156)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D147)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D156)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D147)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D166:D175">
+  <conditionalFormatting sqref="D157:D166">
     <cfRule type="containsText" dxfId="29" priority="37" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D166)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D157)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="28" priority="38" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D166)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D157)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="27" priority="39" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D166)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D157)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D100:D105">
+  <conditionalFormatting sqref="D91:D96">
     <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D91)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D91)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70:D71">
@@ -4740,15 +4618,15 @@
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D70)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D189:D198">
+  <conditionalFormatting sqref="D180:D189">
     <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D189)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D180)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D189)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D180)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D189)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46:D47">
@@ -4773,48 +4651,48 @@
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D205">
+  <conditionalFormatting sqref="D196">
     <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D205)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D196)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D205)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D196)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D205)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D196)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D206">
+  <conditionalFormatting sqref="D197">
     <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D206)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D197)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D206)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D197)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D206)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D197)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D207">
+  <conditionalFormatting sqref="D198">
     <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D207)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D198)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D207)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D198)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D207)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D198)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D208:D214">
+  <conditionalFormatting sqref="D199:D205">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D208)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D199)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D208)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D199)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D208)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D199)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modificación alcance 14.5 Identificación reportes compartidos con el gabinete psicopedagógico
</commit_message>
<xml_diff>
--- a/Docs/04-Requerimientos/Proyecto_Final_Status.xlsx
+++ b/Docs/04-Requerimientos/Proyecto_Final_Status.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="131">
   <si>
     <t>COMPLETADO</t>
   </si>
@@ -295,9 +295,6 @@
     <t>14.4 Consultar tablero de control Directivo: Representación gráfica del nivel de inasistencias de cursos (docentes)</t>
   </si>
   <si>
-    <t>14.5 Generar reporte de alumnos y de profesores según sus inasistencias.</t>
-  </si>
-  <si>
     <t>14.6 Generar reporte de rendimientos de profesores por periodo.</t>
   </si>
   <si>
@@ -428,6 +425,9 @@
   </si>
   <si>
     <t>27- Actividades adicionales</t>
+  </si>
+  <si>
+    <t>14.5 Generar reporte de profesores según sus inasistencias.</t>
   </si>
 </sst>
 </file>
@@ -1296,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,7 +2598,9 @@
     </row>
     <row r="81" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="9"/>
-      <c r="B81" s="9"/>
+      <c r="B81" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="C81" s="24"/>
       <c r="D81" s="14"/>
       <c r="E81" s="5"/>
@@ -2611,7 +2613,9 @@
     </row>
     <row r="82" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="9"/>
-      <c r="B82" s="9"/>
+      <c r="B82" s="29" t="s">
+        <v>79</v>
+      </c>
       <c r="C82" s="24"/>
       <c r="D82" s="14"/>
       <c r="E82" s="5"/>
@@ -2757,7 +2761,7 @@
         <v>26</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="C91" s="24">
         <v>20</v>
@@ -2776,7 +2780,7 @@
         <v>26</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C92" s="24">
         <v>20</v>
@@ -2795,7 +2799,7 @@
         <v>26</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C93" s="24">
         <v>20</v>
@@ -2814,7 +2818,7 @@
         <v>26</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C94" s="24">
         <v>20</v>
@@ -2833,7 +2837,7 @@
         <v>26</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C95" s="24">
         <v>20</v>
@@ -2865,7 +2869,7 @@
         <v>9</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C97" s="21"/>
       <c r="D97" s="12"/>
@@ -2882,7 +2886,7 @@
         <v>9</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C98" s="24">
         <v>18</v>
@@ -2901,7 +2905,7 @@
         <v>9</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C99" s="24">
         <v>14</v>
@@ -2920,7 +2924,7 @@
         <v>9</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C100" s="24">
         <v>12</v>
@@ -3015,7 +3019,7 @@
     <row r="107" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C107" s="21"/>
       <c r="D107" s="12"/>
@@ -3032,7 +3036,7 @@
         <v>9</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C108" s="24">
         <v>18</v>
@@ -3153,7 +3157,7 @@
     <row r="117" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C117" s="21"/>
       <c r="D117" s="12"/>
@@ -3170,7 +3174,7 @@
         <v>9</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C118" s="24">
         <v>20</v>
@@ -3189,7 +3193,7 @@
         <v>9</v>
       </c>
       <c r="B119" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C119" s="26">
         <v>26</v>
@@ -3208,7 +3212,7 @@
         <v>9</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C120" s="24">
         <v>26</v>
@@ -3305,7 +3309,7 @@
         <v>22</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C127" s="21"/>
       <c r="D127" s="12"/>
@@ -3322,7 +3326,7 @@
         <v>44</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C128" s="24">
         <v>18</v>
@@ -3341,7 +3345,7 @@
         <v>44</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C129" s="24">
         <v>18</v>
@@ -3360,7 +3364,7 @@
         <v>44</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C130" s="24">
         <v>18</v>
@@ -3379,7 +3383,7 @@
         <v>44</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C131" s="24">
         <v>18</v>
@@ -3398,7 +3402,7 @@
         <v>44</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C132" s="24">
         <v>18</v>
@@ -3469,7 +3473,7 @@
         <v>22</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C137" s="21"/>
       <c r="D137" s="12"/>
@@ -3486,7 +3490,7 @@
         <v>44</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C138" s="24">
         <v>24</v>
@@ -3505,7 +3509,7 @@
         <v>44</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C139" s="24">
         <v>24</v>
@@ -3524,7 +3528,7 @@
         <v>44</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C140" s="24">
         <v>30</v>
@@ -3621,7 +3625,7 @@
         <v>22</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C147" s="21"/>
       <c r="D147" s="12"/>
@@ -3636,7 +3640,7 @@
     <row r="148" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="9"/>
       <c r="B148" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C148" s="24"/>
       <c r="D148" s="14"/>
@@ -3757,7 +3761,7 @@
         <v>22</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C157" s="21"/>
       <c r="D157" s="12"/>
@@ -3772,7 +3776,7 @@
     <row r="158" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="9"/>
       <c r="B158" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C158" s="24"/>
       <c r="D158" s="14"/>
@@ -3893,7 +3897,7 @@
         <v>22</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C167" s="21"/>
       <c r="D167" s="12"/>
@@ -3908,7 +3912,7 @@
     <row r="168" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="9"/>
       <c r="B168" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C168" s="24"/>
       <c r="D168" s="14"/>
@@ -3964,7 +3968,7 @@
         <v>22</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C172" s="21"/>
       <c r="D172" s="12"/>
@@ -3979,7 +3983,7 @@
     <row r="173" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="9"/>
       <c r="B173" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C173" s="24">
         <v>16</v>
@@ -3996,7 +4000,7 @@
     <row r="174" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="9"/>
       <c r="B174" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C174" s="24">
         <v>16</v>
@@ -4013,7 +4017,7 @@
     <row r="175" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="9"/>
       <c r="B175" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C175" s="24">
         <v>10</v>
@@ -4084,7 +4088,7 @@
         <v>22</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C180" s="21"/>
       <c r="D180" s="12"/>
@@ -4101,7 +4105,7 @@
         <v>45</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C181" s="24">
         <v>12</v>
@@ -4120,7 +4124,7 @@
         <v>45</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C182" s="24">
         <v>12</v>
@@ -4139,7 +4143,7 @@
         <v>45</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C183" s="24">
         <v>12</v>
@@ -4158,7 +4162,7 @@
         <v>45</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C184" s="24">
         <v>12</v>
@@ -4177,7 +4181,7 @@
         <v>45</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C185" s="24">
         <v>12</v>
@@ -4196,7 +4200,7 @@
         <v>45</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C186" s="24">
         <v>12</v>
@@ -4215,7 +4219,7 @@
         <v>45</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C187" s="24">
         <v>12</v>
@@ -4234,7 +4238,7 @@
         <v>45</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C188" s="24">
         <v>12</v>
@@ -4264,7 +4268,7 @@
     <row r="191" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A191" s="9"/>
       <c r="B191" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C191" s="24"/>
       <c r="D191" s="14"/>

</xml_diff>

<commit_message>
Casos de uso asociados al modulo de reportes
</commit_message>
<xml_diff>
--- a/Docs/04-Requerimientos/Proyecto_Final_Status.xlsx
+++ b/Docs/04-Requerimientos/Proyecto_Final_Status.xlsx
@@ -20,12 +20,12 @@
     <definedName name="_Toc220775280" localSheetId="1">Sheet1!$B$41</definedName>
     <definedName name="_Toc220775281" localSheetId="1">Sheet1!$B$48</definedName>
     <definedName name="_Toc220775282" localSheetId="1">Sheet1!$B$55</definedName>
-    <definedName name="_Toc220775283" localSheetId="1">Sheet1!$B$60</definedName>
-    <definedName name="_Toc220775284" localSheetId="1">Sheet1!$B$66</definedName>
-    <definedName name="_Toc220775285" localSheetId="1">Sheet1!$B$74</definedName>
-    <definedName name="_Toc220775286" localSheetId="1">Sheet1!$B$81</definedName>
+    <definedName name="_Toc220775283" localSheetId="1">Sheet1!$B$63</definedName>
+    <definedName name="_Toc220775284" localSheetId="1">Sheet1!$B$69</definedName>
+    <definedName name="_Toc220775285" localSheetId="1">Sheet1!$B$77</definedName>
+    <definedName name="_Toc220775286" localSheetId="1">Sheet1!$B$87</definedName>
     <definedName name="_Toc220775287" localSheetId="1">Sheet1!#REF!</definedName>
-    <definedName name="_Toc220775288" localSheetId="1">Sheet1!$B$87</definedName>
+    <definedName name="_Toc220775288" localSheetId="1">Sheet1!$B$95</definedName>
     <definedName name="_Toc220775289" localSheetId="1">Sheet1!#REF!</definedName>
     <definedName name="_Toc290939942" localSheetId="1">Sheet1!$A$2</definedName>
     <definedName name="_Toc439994688" localSheetId="1">Sheet1!$B$2</definedName>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="175">
   <si>
     <t>COMPLETADO</t>
   </si>
@@ -148,9 +148,6 @@
     <t>11.1 Generar mensaje.</t>
   </si>
   <si>
-    <t>12.3 Generar reporte estadísticos de desempeño de alumnos en diferentes materias en el período respecto a años anteriores.</t>
-  </si>
-  <si>
     <t>Comunicación</t>
   </si>
   <si>
@@ -542,6 +539,51 @@
   </si>
   <si>
     <t>Modulo de gestion de planificacion</t>
+  </si>
+  <si>
+    <t>27. Generar reporte de notas de cada una de las materias en los que va del año de un alumno</t>
+  </si>
+  <si>
+    <t>28. Exportar a PDF</t>
+  </si>
+  <si>
+    <t>29. Imprimir reporte</t>
+  </si>
+  <si>
+    <t>26. Generar reporte estadísticos de desempeño de alumnos en diferentes materias en el período respecto a años anteriores</t>
+  </si>
+  <si>
+    <t>24. Generar reporte estadístico sobre las encuestas de docente</t>
+  </si>
+  <si>
+    <t>25. Generar reporte estadístico sobre las encuestas de docente</t>
+  </si>
+  <si>
+    <t>19. Generar reporte de rendimiento de alumnos por periodo</t>
+  </si>
+  <si>
+    <t>26. Generar reporte estadístico sobre las encuestas de docente</t>
+  </si>
+  <si>
+    <t>18. Generar reporte de profesores según sus inasistencias</t>
+  </si>
+  <si>
+    <t>20. Generar reporte de rendimientos de profesores por periodo</t>
+  </si>
+  <si>
+    <t>21. Generar reporte de rendimiento por cursos</t>
+  </si>
+  <si>
+    <t>22. Generar reporte de rendimiento por asignatura y curso</t>
+  </si>
+  <si>
+    <t>23. Generar reporte estadístico de uso sobre la cantidad de accesos a la autogestión por mes</t>
+  </si>
+  <si>
+    <t>1.1a</t>
+  </si>
+  <si>
+    <t>Modulo de reportes</t>
   </si>
 </sst>
 </file>
@@ -662,7 +704,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -778,11 +820,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -883,9 +938,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -895,6 +947,13 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1536,7 +1595,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,7 +1608,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1557,18 +1616,18 @@
     </row>
     <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>127</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>129</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1580,65 +1639,73 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="C8" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="D8" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="38" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
-        <v>137</v>
+      <c r="A9" s="48" t="s">
+        <v>136</v>
       </c>
       <c r="B9" s="39">
         <v>40678</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
-        <v>158</v>
+      <c r="A10" s="49" t="s">
+        <v>157</v>
       </c>
       <c r="B10" s="39">
         <v>40678</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>160</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="49" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="39">
+        <v>40678</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="40"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="41"/>
       <c r="C13" s="42"/>
       <c r="D13" s="43"/>
@@ -1657,11 +1724,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K211"/>
+  <dimension ref="A1:K229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="675" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="675" topLeftCell="A187" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B202" sqref="B202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,7 +1753,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>2</v>
@@ -1695,13 +1762,13 @@
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>2</v>
@@ -1730,10 +1797,10 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="19">
         <v>16</v>
@@ -1749,10 +1816,10 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="19">
         <v>12</v>
@@ -1768,10 +1835,10 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="19">
         <v>18</v>
@@ -1841,10 +1908,10 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="19">
         <v>10</v>
@@ -1860,10 +1927,10 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="23">
         <v>16</v>
@@ -1933,10 +2000,10 @@
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="C16" s="19">
         <v>24</v>
@@ -1952,10 +2019,10 @@
     </row>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="19">
         <v>18</v>
@@ -1971,10 +2038,10 @@
     </row>
     <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="19">
         <v>18</v>
@@ -1990,10 +2057,10 @@
     </row>
     <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="19">
         <v>18</v>
@@ -2009,10 +2076,10 @@
     </row>
     <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="19">
         <v>18</v>
@@ -2028,10 +2095,10 @@
     </row>
     <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="19">
         <v>14</v>
@@ -2088,10 +2155,10 @@
     </row>
     <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="24">
         <v>16</v>
@@ -2107,10 +2174,10 @@
     </row>
     <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="24">
         <v>12</v>
@@ -2183,13 +2250,15 @@
         <v>26</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="24">
         <v>20</v>
       </c>
       <c r="D31" s="14"/>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -2202,7 +2271,9 @@
       <c r="B32" s="9"/>
       <c r="C32" s="24"/>
       <c r="D32" s="14"/>
-      <c r="E32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
@@ -2215,7 +2286,9 @@
       <c r="B33" s="9"/>
       <c r="C33" s="24"/>
       <c r="D33" s="14"/>
-      <c r="E33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
@@ -2269,13 +2342,15 @@
         <v>26</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="25">
         <v>25</v>
       </c>
       <c r="D37" s="14"/>
-      <c r="E37" s="5"/>
+      <c r="E37" s="5" t="s">
+        <v>163</v>
+      </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
@@ -2288,7 +2363,9 @@
       <c r="B38" s="9"/>
       <c r="C38" s="24"/>
       <c r="D38" s="14"/>
-      <c r="E38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
@@ -2301,7 +2378,9 @@
       <c r="B39" s="9"/>
       <c r="C39" s="24"/>
       <c r="D39" s="14"/>
-      <c r="E39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
@@ -2339,10 +2418,10 @@
     </row>
     <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C42" s="24">
         <v>40</v>
@@ -2358,10 +2437,10 @@
     </row>
     <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="C43" s="24">
         <v>12</v>
@@ -2377,10 +2456,10 @@
     </row>
     <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" s="24">
         <v>20</v>
@@ -2396,10 +2475,10 @@
     </row>
     <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="24">
         <v>10</v>
@@ -2456,10 +2535,10 @@
     </row>
     <row r="49" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" s="24">
         <v>40</v>
@@ -2475,10 +2554,10 @@
     </row>
     <row r="50" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" s="24">
         <v>10</v>
@@ -2494,10 +2573,10 @@
     </row>
     <row r="51" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" s="24">
         <v>20</v>
@@ -2513,10 +2592,10 @@
     </row>
     <row r="52" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52" s="24">
         <v>10</v>
@@ -2576,13 +2655,15 @@
         <v>26</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C56" s="24">
         <v>25</v>
       </c>
       <c r="D56" s="14"/>
-      <c r="E56" s="5"/>
+      <c r="E56" s="5" t="s">
+        <v>164</v>
+      </c>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
@@ -2591,15 +2672,13 @@
       <c r="K56" s="5"/>
     </row>
     <row r="57" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>80</v>
-      </c>
+      <c r="A57" s="9"/>
+      <c r="B57" s="29"/>
       <c r="C57" s="24"/>
       <c r="D57" s="14"/>
-      <c r="E57" s="5"/>
+      <c r="E57" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
@@ -2609,10 +2688,12 @@
     </row>
     <row r="58" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
-      <c r="B58" s="9"/>
+      <c r="B58" s="29"/>
       <c r="C58" s="24"/>
       <c r="D58" s="14"/>
-      <c r="E58" s="5"/>
+      <c r="E58" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
@@ -2620,12 +2701,18 @@
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="22"/>
+    <row r="59" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" s="24"/>
       <c r="D59" s="14"/>
-      <c r="E59" s="5"/>
+      <c r="E59" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
@@ -2633,33 +2720,29 @@
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
     </row>
-    <row r="60" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C60" s="21"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
-      <c r="H60" s="10"/>
-      <c r="I60" s="10"/>
-      <c r="J60" s="10"/>
-      <c r="K60" s="10"/>
+    <row r="60" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
     </row>
     <row r="61" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C61" s="24">
-        <v>20</v>
-      </c>
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="24"/>
       <c r="D61" s="14"/>
-      <c r="E61" s="5"/>
+      <c r="E61" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
@@ -2667,16 +2750,10 @@
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
     </row>
-    <row r="62" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C62" s="24">
-        <v>20</v>
-      </c>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="22"/>
       <c r="D62" s="14"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -2686,23 +2763,31 @@
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
     </row>
-    <row r="63" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="B63" s="6"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
+    <row r="63" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" s="21"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10"/>
+      <c r="K63" s="10"/>
     </row>
     <row r="64" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" s="6"/>
-      <c r="C64" s="19"/>
+      <c r="A64" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C64" s="24">
+        <v>20</v>
+      </c>
       <c r="D64" s="14"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
@@ -2712,10 +2797,16 @@
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="22"/>
+    <row r="65" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C65" s="24">
+        <v>20</v>
+      </c>
       <c r="D65" s="14"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
@@ -2725,31 +2816,23 @@
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
     </row>
-    <row r="66" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C66" s="21"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="10"/>
-      <c r="H66" s="10"/>
-      <c r="I66" s="10"/>
-      <c r="J66" s="10"/>
-      <c r="K66" s="10"/>
+    <row r="66" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="6"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
     </row>
     <row r="67" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C67" s="24">
-        <v>12</v>
-      </c>
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="19"/>
       <c r="D67" s="14"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
@@ -2759,16 +2842,10 @@
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
     </row>
-    <row r="68" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C68" s="24">
-        <v>15</v>
-      </c>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="22"/>
       <c r="D68" s="14"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
@@ -2778,29 +2855,31 @@
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
     </row>
-    <row r="69" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C69" s="24">
-        <v>10</v>
-      </c>
-      <c r="D69" s="14"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
+    <row r="69" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="21"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
     </row>
     <row r="70" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="9"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="24"/>
+      <c r="A70" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C70" s="24">
+        <v>12</v>
+      </c>
       <c r="D70" s="14"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -2811,9 +2890,15 @@
       <c r="K70" s="5"/>
     </row>
     <row r="71" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="9"/>
-      <c r="B71" s="9"/>
-      <c r="C71" s="24"/>
+      <c r="A71" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71" s="24">
+        <v>15</v>
+      </c>
       <c r="D71" s="14"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
@@ -2824,9 +2909,15 @@
       <c r="K71" s="5"/>
     </row>
     <row r="72" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="9"/>
-      <c r="B72" s="9"/>
-      <c r="C72" s="24"/>
+      <c r="A72" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C72" s="24">
+        <v>10</v>
+      </c>
       <c r="D72" s="14"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
@@ -2836,10 +2927,10 @@
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="22"/>
+    <row r="73" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="24"/>
       <c r="D73" s="14"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
@@ -2849,35 +2940,25 @@
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
     </row>
-    <row r="74" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C74" s="21"/>
-      <c r="D74" s="12"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="10"/>
-      <c r="G74" s="10"/>
-      <c r="H74" s="10"/>
-      <c r="I74" s="10"/>
-      <c r="J74" s="10"/>
-      <c r="K74" s="10"/>
+    <row r="74" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="24"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
     </row>
     <row r="75" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C75" s="23">
-        <v>15</v>
-      </c>
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="24"/>
       <c r="D75" s="14"/>
-      <c r="E75" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="E75" s="5"/>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
@@ -2885,14 +2966,12 @@
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
     </row>
-    <row r="76" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="9"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="23"/>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="22"/>
       <c r="D76" s="14"/>
-      <c r="E76" s="5" t="s">
-        <v>150</v>
-      </c>
+      <c r="E76" s="5"/>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
@@ -2900,37 +2979,35 @@
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
     </row>
-    <row r="77" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C77" s="19">
-        <v>22</v>
-      </c>
-      <c r="D77" s="14"/>
-      <c r="E77" s="16"/>
-      <c r="F77" s="16"/>
-      <c r="G77" s="16"/>
-      <c r="H77" s="16"/>
-      <c r="I77" s="16"/>
-      <c r="J77" s="16"/>
-      <c r="K77" s="16"/>
+    <row r="77" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77" s="21"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+      <c r="J77" s="10"/>
+      <c r="K77" s="10"/>
     </row>
     <row r="78" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C78" s="19">
-        <v>22</v>
+      <c r="A78" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C78" s="23">
+        <v>15</v>
       </c>
       <c r="D78" s="14"/>
-      <c r="E78" s="5"/>
+      <c r="E78" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
@@ -2939,73 +3016,85 @@
       <c r="K78" s="5"/>
     </row>
     <row r="79" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
-      <c r="B79" s="6"/>
-      <c r="C79" s="19"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="23"/>
       <c r="D79" s="14"/>
-      <c r="E79" s="16"/>
-      <c r="F79" s="16"/>
-      <c r="G79" s="16"/>
-      <c r="H79" s="16"/>
-      <c r="I79" s="16"/>
-      <c r="J79" s="16"/>
-      <c r="K79" s="16"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="22"/>
+      <c r="E79" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+    </row>
+    <row r="80" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C80" s="19">
+        <v>22</v>
+      </c>
       <c r="D80" s="14"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
-      <c r="J80" s="5"/>
-      <c r="K80" s="5"/>
-    </row>
-    <row r="81" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C81" s="21"/>
-      <c r="D81" s="12"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="10"/>
-      <c r="G81" s="10"/>
-      <c r="H81" s="10"/>
-      <c r="I81" s="10"/>
-      <c r="J81" s="10"/>
-      <c r="K81" s="10"/>
+      <c r="E80" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F80" s="16"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="16"/>
+      <c r="I80" s="16"/>
+      <c r="J80" s="16"/>
+      <c r="K80" s="16"/>
+    </row>
+    <row r="81" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F81" s="16"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
+      <c r="J81" s="16"/>
+      <c r="K81" s="16"/>
     </row>
     <row r="82" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C82" s="24"/>
+      <c r="A82" s="6"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="19"/>
       <c r="D82" s="14"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
-      <c r="I82" s="5"/>
-      <c r="J82" s="5"/>
-      <c r="K82" s="5"/>
+      <c r="E82" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F82" s="16"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+      <c r="J82" s="16"/>
+      <c r="K82" s="16"/>
     </row>
     <row r="83" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B83" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C83" s="24"/>
+      <c r="B83" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C83" s="19">
+        <v>22</v>
+      </c>
       <c r="D83" s="14"/>
-      <c r="E83" s="5"/>
+      <c r="E83" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
@@ -3014,11 +3103,13 @@
       <c r="K83" s="5"/>
     </row>
     <row r="84" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="9"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="24"/>
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="19"/>
       <c r="D84" s="14"/>
-      <c r="E84" s="5"/>
+      <c r="E84" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
@@ -3027,22 +3118,24 @@
       <c r="K84" s="5"/>
     </row>
     <row r="85" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="9"/>
-      <c r="B85" s="9"/>
-      <c r="C85" s="24"/>
+      <c r="A85" s="6"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="19"/>
       <c r="D85" s="14"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="5"/>
-      <c r="H85" s="5"/>
-      <c r="I85" s="5"/>
-      <c r="J85" s="5"/>
-      <c r="K85" s="5"/>
-    </row>
-    <row r="86" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="9"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="24"/>
+      <c r="E85" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F85" s="16"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="16"/>
+      <c r="I85" s="16"/>
+      <c r="J85" s="16"/>
+      <c r="K85" s="16"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="22"/>
       <c r="D86" s="14"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
@@ -3055,7 +3148,7 @@
     <row r="87" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C87" s="21"/>
       <c r="D87" s="12"/>
@@ -3068,18 +3161,16 @@
       <c r="K87" s="10"/>
     </row>
     <row r="88" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B88" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C88" s="26">
-        <v>12</v>
-      </c>
+      <c r="A88" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="C88" s="24"/>
       <c r="D88" s="14"/>
       <c r="E88" s="5" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="F88" s="5"/>
       <c r="G88" s="5"/>
@@ -3089,12 +3180,12 @@
       <c r="K88" s="5"/>
     </row>
     <row r="89" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="9"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="26"/>
+      <c r="A89" s="6"/>
+      <c r="B89" s="51"/>
+      <c r="C89" s="24"/>
       <c r="D89" s="14"/>
       <c r="E89" s="5" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
@@ -3104,18 +3195,12 @@
       <c r="K89" s="5"/>
     </row>
     <row r="90" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C90" s="24">
-        <v>12</v>
-      </c>
+      <c r="A90" s="6"/>
+      <c r="B90" s="18"/>
+      <c r="C90" s="24"/>
       <c r="D90" s="14"/>
       <c r="E90" s="5" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
@@ -3125,12 +3210,16 @@
       <c r="K90" s="5"/>
     </row>
     <row r="91" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="9"/>
-      <c r="B91" s="9"/>
+      <c r="A91" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91" s="29" t="s">
+        <v>78</v>
+      </c>
       <c r="C91" s="24"/>
       <c r="D91" s="14"/>
       <c r="E91" s="5" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -3140,18 +3229,12 @@
       <c r="K91" s="5"/>
     </row>
     <row r="92" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B92" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C92" s="24">
-        <v>12</v>
-      </c>
+      <c r="A92" s="9"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="24"/>
       <c r="D92" s="14"/>
       <c r="E92" s="5" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
@@ -3166,7 +3249,7 @@
       <c r="C93" s="24"/>
       <c r="D93" s="14"/>
       <c r="E93" s="5" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
@@ -3176,19 +3259,11 @@
       <c r="K93" s="5"/>
     </row>
     <row r="94" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C94" s="24">
-        <v>12</v>
-      </c>
+      <c r="A94" s="9"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="24"/>
       <c r="D94" s="14"/>
-      <c r="E94" s="5" t="s">
-        <v>151</v>
-      </c>
+      <c r="E94" s="5"/>
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
       <c r="H94" s="5"/>
@@ -3196,33 +3271,35 @@
       <c r="J94" s="5"/>
       <c r="K94" s="5"/>
     </row>
-    <row r="95" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="9"/>
-      <c r="B95" s="9"/>
-      <c r="C95" s="24"/>
-      <c r="D95" s="14"/>
-      <c r="E95" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5"/>
-      <c r="H95" s="5"/>
-      <c r="I95" s="5"/>
-      <c r="J95" s="5"/>
-      <c r="K95" s="5"/>
+    <row r="95" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C95" s="21"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="10"/>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
+      <c r="J95" s="10"/>
+      <c r="K95" s="10"/>
     </row>
     <row r="96" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C96" s="24">
-        <v>20</v>
+        <v>9</v>
+      </c>
+      <c r="B96" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C96" s="26">
+        <v>12</v>
       </c>
       <c r="D96" s="14"/>
-      <c r="E96" s="5"/>
+      <c r="E96" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="F96" s="5"/>
       <c r="G96" s="5"/>
       <c r="H96" s="5"/>
@@ -3231,17 +3308,13 @@
       <c r="K96" s="5"/>
     </row>
     <row r="97" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C97" s="24">
-        <v>20</v>
-      </c>
+      <c r="A97" s="9"/>
+      <c r="B97" s="17"/>
+      <c r="C97" s="26"/>
       <c r="D97" s="14"/>
-      <c r="E97" s="5"/>
+      <c r="E97" s="5" t="s">
+        <v>151</v>
+      </c>
       <c r="F97" s="5"/>
       <c r="G97" s="5"/>
       <c r="H97" s="5"/>
@@ -3251,16 +3324,18 @@
     </row>
     <row r="98" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C98" s="24">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D98" s="14"/>
-      <c r="E98" s="5"/>
+      <c r="E98" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
       <c r="H98" s="5"/>
@@ -3269,17 +3344,13 @@
       <c r="K98" s="5"/>
     </row>
     <row r="99" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C99" s="24">
-        <v>20</v>
-      </c>
+      <c r="A99" s="9"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="24"/>
       <c r="D99" s="14"/>
-      <c r="E99" s="5"/>
+      <c r="E99" s="5" t="s">
+        <v>152</v>
+      </c>
       <c r="F99" s="5"/>
       <c r="G99" s="5"/>
       <c r="H99" s="5"/>
@@ -3289,16 +3360,18 @@
     </row>
     <row r="100" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C100" s="24">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D100" s="14"/>
-      <c r="E100" s="5"/>
+      <c r="E100" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
       <c r="H100" s="5"/>
@@ -3311,7 +3384,9 @@
       <c r="B101" s="9"/>
       <c r="C101" s="24"/>
       <c r="D101" s="14"/>
-      <c r="E101" s="5"/>
+      <c r="E101" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
       <c r="H101" s="5"/>
@@ -3319,36 +3394,34 @@
       <c r="J101" s="5"/>
       <c r="K101" s="5"/>
     </row>
-    <row r="102" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
+    <row r="102" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B102" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C102" s="21"/>
-      <c r="D102" s="12"/>
-      <c r="E102" s="10"/>
-      <c r="F102" s="10"/>
-      <c r="G102" s="10"/>
-      <c r="H102" s="10"/>
-      <c r="I102" s="10"/>
-      <c r="J102" s="10"/>
-      <c r="K102" s="10"/>
+      <c r="B102" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C102" s="24">
+        <v>12</v>
+      </c>
+      <c r="D102" s="14"/>
+      <c r="E102" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="5"/>
+      <c r="J102" s="5"/>
+      <c r="K102" s="5"/>
     </row>
     <row r="103" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C103" s="24">
-        <v>18</v>
-      </c>
+      <c r="A103" s="9"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="24"/>
       <c r="D103" s="14"/>
-      <c r="E103" s="48" t="s">
-        <v>142</v>
+      <c r="E103" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
@@ -3358,12 +3431,18 @@
       <c r="K103" s="5"/>
     </row>
     <row r="104" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="9"/>
-      <c r="B104" s="9"/>
-      <c r="C104" s="24"/>
+      <c r="A104" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C104" s="24">
+        <v>20</v>
+      </c>
       <c r="D104" s="14"/>
-      <c r="E104" s="48" t="s">
-        <v>143</v>
+      <c r="E104" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
@@ -3377,8 +3456,8 @@
       <c r="B105" s="9"/>
       <c r="C105" s="24"/>
       <c r="D105" s="14"/>
-      <c r="E105" s="48" t="s">
-        <v>144</v>
+      <c r="E105" s="5" t="s">
+        <v>161</v>
       </c>
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
@@ -3392,6 +3471,9 @@
       <c r="B106" s="9"/>
       <c r="C106" s="24"/>
       <c r="D106" s="14"/>
+      <c r="E106" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
       <c r="H106" s="5"/>
@@ -3400,11 +3482,19 @@
       <c r="K106" s="5"/>
     </row>
     <row r="107" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="9"/>
-      <c r="B107" s="9"/>
-      <c r="C107" s="24"/>
+      <c r="A107" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C107" s="24">
+        <v>20</v>
+      </c>
       <c r="D107" s="14"/>
-      <c r="E107" s="5"/>
+      <c r="E107" s="5" t="s">
+        <v>169</v>
+      </c>
       <c r="F107" s="5"/>
       <c r="G107" s="5"/>
       <c r="H107" s="5"/>
@@ -3417,6 +3507,9 @@
       <c r="B108" s="9"/>
       <c r="C108" s="24"/>
       <c r="D108" s="14"/>
+      <c r="E108" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="F108" s="5"/>
       <c r="G108" s="5"/>
       <c r="H108" s="5"/>
@@ -3429,7 +3522,9 @@
       <c r="B109" s="9"/>
       <c r="C109" s="24"/>
       <c r="D109" s="14"/>
-      <c r="E109" s="5"/>
+      <c r="E109" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="F109" s="5"/>
       <c r="G109" s="5"/>
       <c r="H109" s="5"/>
@@ -3438,11 +3533,19 @@
       <c r="K109" s="5"/>
     </row>
     <row r="110" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="9"/>
-      <c r="B110" s="9"/>
-      <c r="C110" s="24"/>
+      <c r="A110" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C110" s="24">
+        <v>20</v>
+      </c>
       <c r="D110" s="14"/>
-      <c r="E110" s="5"/>
+      <c r="E110" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="F110" s="5"/>
       <c r="G110" s="5"/>
       <c r="H110" s="5"/>
@@ -3450,34 +3553,28 @@
       <c r="J110" s="5"/>
       <c r="K110" s="5"/>
     </row>
-    <row r="111" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A111" s="4"/>
-      <c r="B111" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C111" s="21"/>
-      <c r="D111" s="12"/>
-      <c r="E111" s="10"/>
-      <c r="F111" s="10"/>
-      <c r="G111" s="10"/>
-      <c r="H111" s="10"/>
-      <c r="I111" s="10"/>
-      <c r="J111" s="10"/>
-      <c r="K111" s="10"/>
+    <row r="111" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="9"/>
+      <c r="B111" s="9"/>
+      <c r="C111" s="24"/>
+      <c r="D111" s="14"/>
+      <c r="E111" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F111" s="5"/>
+      <c r="G111" s="5"/>
+      <c r="H111" s="5"/>
+      <c r="I111" s="5"/>
+      <c r="J111" s="5"/>
+      <c r="K111" s="5"/>
     </row>
     <row r="112" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B112" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="C112" s="24">
-        <v>18</v>
-      </c>
+      <c r="A112" s="9"/>
+      <c r="B112" s="9"/>
+      <c r="C112" s="24"/>
       <c r="D112" s="14"/>
       <c r="E112" s="5" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
@@ -3487,12 +3584,18 @@
       <c r="K112" s="5"/>
     </row>
     <row r="113" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="9"/>
-      <c r="B113" s="9"/>
-      <c r="C113" s="24"/>
+      <c r="A113" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C113" s="24">
+        <v>20</v>
+      </c>
       <c r="D113" s="14"/>
       <c r="E113" s="5" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
@@ -3507,7 +3610,7 @@
       <c r="C114" s="24"/>
       <c r="D114" s="14"/>
       <c r="E114" s="5" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="F114" s="5"/>
       <c r="G114" s="5"/>
@@ -3521,7 +3624,9 @@
       <c r="B115" s="9"/>
       <c r="C115" s="24"/>
       <c r="D115" s="14"/>
-      <c r="E115" s="5"/>
+      <c r="E115" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="F115" s="5"/>
       <c r="G115" s="5"/>
       <c r="H115" s="5"/>
@@ -3530,11 +3635,19 @@
       <c r="K115" s="5"/>
     </row>
     <row r="116" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A116" s="9"/>
-      <c r="B116" s="9"/>
-      <c r="C116" s="24"/>
+      <c r="A116" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C116" s="24">
+        <v>20</v>
+      </c>
       <c r="D116" s="14"/>
-      <c r="E116" s="5"/>
+      <c r="E116" s="5" t="s">
+        <v>172</v>
+      </c>
       <c r="F116" s="5"/>
       <c r="G116" s="5"/>
       <c r="H116" s="5"/>
@@ -3547,7 +3660,9 @@
       <c r="B117" s="9"/>
       <c r="C117" s="24"/>
       <c r="D117" s="14"/>
-      <c r="E117" s="5"/>
+      <c r="E117" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
       <c r="H117" s="5"/>
@@ -3560,7 +3675,9 @@
       <c r="B118" s="9"/>
       <c r="C118" s="24"/>
       <c r="D118" s="14"/>
-      <c r="E118" s="5"/>
+      <c r="E118" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
       <c r="H118" s="5"/>
@@ -3581,47 +3698,51 @@
       <c r="J119" s="5"/>
       <c r="K119" s="5"/>
     </row>
-    <row r="120" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="9"/>
-      <c r="B120" s="9"/>
-      <c r="C120" s="24"/>
-      <c r="D120" s="14"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
-      <c r="G120" s="5"/>
-      <c r="H120" s="5"/>
-      <c r="I120" s="5"/>
-      <c r="J120" s="5"/>
-      <c r="K120" s="5"/>
-    </row>
-    <row r="121" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A121" s="4"/>
-      <c r="B121" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C121" s="21"/>
-      <c r="D121" s="12"/>
-      <c r="E121" s="10"/>
-      <c r="F121" s="10"/>
-      <c r="G121" s="10"/>
-      <c r="H121" s="10"/>
-      <c r="I121" s="10"/>
-      <c r="J121" s="10"/>
-      <c r="K121" s="10"/>
+    <row r="120" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A120" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C120" s="21"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="10"/>
+      <c r="F120" s="10"/>
+      <c r="G120" s="10"/>
+      <c r="H120" s="10"/>
+      <c r="I120" s="10"/>
+      <c r="J120" s="10"/>
+      <c r="K120" s="10"/>
+    </row>
+    <row r="121" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A121" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C121" s="24">
+        <v>18</v>
+      </c>
+      <c r="D121" s="14"/>
+      <c r="E121" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="F121" s="5"/>
+      <c r="G121" s="5"/>
+      <c r="H121" s="5"/>
+      <c r="I121" s="5"/>
+      <c r="J121" s="5"/>
+      <c r="K121" s="5"/>
     </row>
     <row r="122" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A122" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C122" s="24">
-        <v>20</v>
-      </c>
+      <c r="A122" s="9"/>
+      <c r="B122" s="9"/>
+      <c r="C122" s="24"/>
       <c r="D122" s="14"/>
-      <c r="E122" s="5" t="s">
-        <v>148</v>
+      <c r="E122" s="52" t="s">
+        <v>142</v>
       </c>
       <c r="F122" s="5"/>
       <c r="G122" s="5"/>
@@ -3631,18 +3752,12 @@
       <c r="K122" s="5"/>
     </row>
     <row r="123" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A123" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B123" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C123" s="26">
-        <v>26</v>
-      </c>
+      <c r="A123" s="9"/>
+      <c r="B123" s="9"/>
+      <c r="C123" s="24"/>
       <c r="D123" s="14"/>
-      <c r="E123" s="5" t="s">
-        <v>149</v>
+      <c r="E123" s="52" t="s">
+        <v>143</v>
       </c>
       <c r="F123" s="5"/>
       <c r="G123" s="5"/>
@@ -3653,12 +3768,9 @@
     </row>
     <row r="124" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="9"/>
-      <c r="B124" s="17"/>
-      <c r="C124" s="26"/>
+      <c r="B124" s="9"/>
+      <c r="C124" s="24"/>
       <c r="D124" s="14"/>
-      <c r="E124" s="5" t="s">
-        <v>157</v>
-      </c>
       <c r="F124" s="5"/>
       <c r="G124" s="5"/>
       <c r="H124" s="5"/>
@@ -3667,19 +3779,11 @@
       <c r="K124" s="5"/>
     </row>
     <row r="125" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A125" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B125" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C125" s="24">
-        <v>26</v>
-      </c>
+      <c r="A125" s="9"/>
+      <c r="B125" s="9"/>
+      <c r="C125" s="24"/>
       <c r="D125" s="14"/>
-      <c r="E125" s="5" t="s">
-        <v>151</v>
-      </c>
+      <c r="E125" s="5"/>
       <c r="F125" s="5"/>
       <c r="G125" s="5"/>
       <c r="H125" s="5"/>
@@ -3692,9 +3796,6 @@
       <c r="B126" s="9"/>
       <c r="C126" s="24"/>
       <c r="D126" s="14"/>
-      <c r="E126" s="5" t="s">
-        <v>156</v>
-      </c>
       <c r="F126" s="5"/>
       <c r="G126" s="5"/>
       <c r="H126" s="5"/>
@@ -3728,25 +3829,35 @@
       <c r="J128" s="5"/>
       <c r="K128" s="5"/>
     </row>
-    <row r="129" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A129" s="9"/>
-      <c r="B129" s="9"/>
-      <c r="C129" s="24"/>
-      <c r="D129" s="14"/>
-      <c r="E129" s="5"/>
-      <c r="F129" s="5"/>
-      <c r="G129" s="5"/>
-      <c r="H129" s="5"/>
-      <c r="I129" s="5"/>
-      <c r="J129" s="5"/>
-      <c r="K129" s="5"/>
+    <row r="129" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C129" s="21"/>
+      <c r="D129" s="12"/>
+      <c r="E129" s="10"/>
+      <c r="F129" s="10"/>
+      <c r="G129" s="10"/>
+      <c r="H129" s="10"/>
+      <c r="I129" s="10"/>
+      <c r="J129" s="10"/>
+      <c r="K129" s="10"/>
     </row>
     <row r="130" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A130" s="9"/>
-      <c r="B130" s="9"/>
-      <c r="C130" s="24"/>
+      <c r="A130" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C130" s="24">
+        <v>18</v>
+      </c>
       <c r="D130" s="14"/>
-      <c r="E130" s="5"/>
+      <c r="E130" s="5" t="s">
+        <v>144</v>
+      </c>
       <c r="F130" s="5"/>
       <c r="G130" s="5"/>
       <c r="H130" s="5"/>
@@ -3759,7 +3870,9 @@
       <c r="B131" s="9"/>
       <c r="C131" s="24"/>
       <c r="D131" s="14"/>
-      <c r="E131" s="5"/>
+      <c r="E131" s="5" t="s">
+        <v>145</v>
+      </c>
       <c r="F131" s="5"/>
       <c r="G131" s="5"/>
       <c r="H131" s="5"/>
@@ -3767,33 +3880,25 @@
       <c r="J131" s="5"/>
       <c r="K131" s="5"/>
     </row>
-    <row r="132" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A132" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C132" s="21"/>
-      <c r="D132" s="12"/>
-      <c r="E132" s="10"/>
-      <c r="F132" s="10"/>
-      <c r="G132" s="10"/>
-      <c r="H132" s="10"/>
-      <c r="I132" s="10"/>
-      <c r="J132" s="10"/>
-      <c r="K132" s="10"/>
+    <row r="132" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A132" s="9"/>
+      <c r="B132" s="9"/>
+      <c r="C132" s="24"/>
+      <c r="D132" s="14"/>
+      <c r="E132" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F132" s="5"/>
+      <c r="G132" s="5"/>
+      <c r="H132" s="5"/>
+      <c r="I132" s="5"/>
+      <c r="J132" s="5"/>
+      <c r="K132" s="5"/>
     </row>
     <row r="133" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B133" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C133" s="24">
-        <v>18</v>
-      </c>
+      <c r="A133" s="9"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="24"/>
       <c r="D133" s="14"/>
       <c r="E133" s="5"/>
       <c r="F133" s="5"/>
@@ -3804,15 +3909,9 @@
       <c r="K133" s="5"/>
     </row>
     <row r="134" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A134" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B134" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C134" s="24">
-        <v>18</v>
-      </c>
+      <c r="A134" s="9"/>
+      <c r="B134" s="9"/>
+      <c r="C134" s="24"/>
       <c r="D134" s="14"/>
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
@@ -3823,15 +3922,9 @@
       <c r="K134" s="5"/>
     </row>
     <row r="135" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A135" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B135" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C135" s="24">
-        <v>18</v>
-      </c>
+      <c r="A135" s="9"/>
+      <c r="B135" s="9"/>
+      <c r="C135" s="24"/>
       <c r="D135" s="14"/>
       <c r="E135" s="5"/>
       <c r="F135" s="5"/>
@@ -3842,15 +3935,9 @@
       <c r="K135" s="5"/>
     </row>
     <row r="136" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A136" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B136" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C136" s="24">
-        <v>18</v>
-      </c>
+      <c r="A136" s="9"/>
+      <c r="B136" s="9"/>
+      <c r="C136" s="24"/>
       <c r="D136" s="14"/>
       <c r="E136" s="5"/>
       <c r="F136" s="5"/>
@@ -3861,15 +3948,9 @@
       <c r="K136" s="5"/>
     </row>
     <row r="137" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A137" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B137" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C137" s="24">
-        <v>18</v>
-      </c>
+      <c r="A137" s="9"/>
+      <c r="B137" s="9"/>
+      <c r="C137" s="24"/>
       <c r="D137" s="14"/>
       <c r="E137" s="5"/>
       <c r="F137" s="5"/>
@@ -3892,25 +3973,35 @@
       <c r="J138" s="5"/>
       <c r="K138" s="5"/>
     </row>
-    <row r="139" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A139" s="9"/>
-      <c r="B139" s="9"/>
-      <c r="C139" s="24"/>
-      <c r="D139" s="14"/>
-      <c r="E139" s="5"/>
-      <c r="F139" s="5"/>
-      <c r="G139" s="5"/>
-      <c r="H139" s="5"/>
-      <c r="I139" s="5"/>
-      <c r="J139" s="5"/>
-      <c r="K139" s="5"/>
+    <row r="139" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A139" s="4"/>
+      <c r="B139" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C139" s="21"/>
+      <c r="D139" s="12"/>
+      <c r="E139" s="10"/>
+      <c r="F139" s="10"/>
+      <c r="G139" s="10"/>
+      <c r="H139" s="10"/>
+      <c r="I139" s="10"/>
+      <c r="J139" s="10"/>
+      <c r="K139" s="10"/>
     </row>
     <row r="140" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A140" s="9"/>
-      <c r="B140" s="9"/>
-      <c r="C140" s="24"/>
+      <c r="A140" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C140" s="24">
+        <v>20</v>
+      </c>
       <c r="D140" s="14"/>
-      <c r="E140" s="5"/>
+      <c r="E140" s="5" t="s">
+        <v>147</v>
+      </c>
       <c r="F140" s="5"/>
       <c r="G140" s="5"/>
       <c r="H140" s="5"/>
@@ -3919,11 +4010,19 @@
       <c r="K140" s="5"/>
     </row>
     <row r="141" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A141" s="9"/>
-      <c r="B141" s="9"/>
-      <c r="C141" s="24"/>
+      <c r="A141" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B141" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C141" s="26">
+        <v>26</v>
+      </c>
       <c r="D141" s="14"/>
-      <c r="E141" s="5"/>
+      <c r="E141" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="F141" s="5"/>
       <c r="G141" s="5"/>
       <c r="H141" s="5"/>
@@ -3931,35 +4030,35 @@
       <c r="J141" s="5"/>
       <c r="K141" s="5"/>
     </row>
-    <row r="142" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A142" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C142" s="21"/>
-      <c r="D142" s="12"/>
-      <c r="E142" s="10"/>
-      <c r="F142" s="10"/>
-      <c r="G142" s="10"/>
-      <c r="H142" s="10"/>
-      <c r="I142" s="10"/>
-      <c r="J142" s="10"/>
-      <c r="K142" s="10"/>
+    <row r="142" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A142" s="9"/>
+      <c r="B142" s="17"/>
+      <c r="C142" s="26"/>
+      <c r="D142" s="14"/>
+      <c r="E142" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F142" s="5"/>
+      <c r="G142" s="5"/>
+      <c r="H142" s="5"/>
+      <c r="I142" s="5"/>
+      <c r="J142" s="5"/>
+      <c r="K142" s="5"/>
     </row>
     <row r="143" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="9" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C143" s="24">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D143" s="14"/>
-      <c r="E143" s="5"/>
+      <c r="E143" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="F143" s="5"/>
       <c r="G143" s="5"/>
       <c r="H143" s="5"/>
@@ -3968,17 +4067,13 @@
       <c r="K143" s="5"/>
     </row>
     <row r="144" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A144" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B144" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C144" s="24">
-        <v>24</v>
-      </c>
+      <c r="A144" s="9"/>
+      <c r="B144" s="9"/>
+      <c r="C144" s="24"/>
       <c r="D144" s="14"/>
-      <c r="E144" s="5"/>
+      <c r="E144" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="F144" s="5"/>
       <c r="G144" s="5"/>
       <c r="H144" s="5"/>
@@ -3987,15 +4082,9 @@
       <c r="K144" s="5"/>
     </row>
     <row r="145" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A145" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B145" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C145" s="24">
-        <v>30</v>
-      </c>
+      <c r="A145" s="9"/>
+      <c r="B145" s="9"/>
+      <c r="C145" s="24"/>
       <c r="D145" s="14"/>
       <c r="E145" s="5"/>
       <c r="F145" s="5"/>
@@ -4057,23 +4146,33 @@
       <c r="J149" s="5"/>
       <c r="K149" s="5"/>
     </row>
-    <row r="150" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" s="9"/>
-      <c r="B150" s="9"/>
-      <c r="C150" s="24"/>
-      <c r="D150" s="14"/>
-      <c r="E150" s="5"/>
-      <c r="F150" s="5"/>
-      <c r="G150" s="5"/>
-      <c r="H150" s="5"/>
-      <c r="I150" s="5"/>
-      <c r="J150" s="5"/>
-      <c r="K150" s="5"/>
+    <row r="150" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A150" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C150" s="21"/>
+      <c r="D150" s="12"/>
+      <c r="E150" s="10"/>
+      <c r="F150" s="10"/>
+      <c r="G150" s="10"/>
+      <c r="H150" s="10"/>
+      <c r="I150" s="10"/>
+      <c r="J150" s="10"/>
+      <c r="K150" s="10"/>
     </row>
     <row r="151" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="9"/>
-      <c r="B151" s="9"/>
-      <c r="C151" s="24"/>
+      <c r="A151" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C151" s="24">
+        <v>18</v>
+      </c>
       <c r="D151" s="14"/>
       <c r="E151" s="5"/>
       <c r="F151" s="5"/>
@@ -4083,29 +4182,35 @@
       <c r="J151" s="5"/>
       <c r="K151" s="5"/>
     </row>
-    <row r="152" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A152" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B152" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C152" s="21"/>
-      <c r="D152" s="12"/>
-      <c r="E152" s="10"/>
-      <c r="F152" s="10"/>
-      <c r="G152" s="10"/>
-      <c r="H152" s="10"/>
-      <c r="I152" s="10"/>
-      <c r="J152" s="10"/>
-      <c r="K152" s="10"/>
+    <row r="152" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A152" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C152" s="24">
+        <v>18</v>
+      </c>
+      <c r="D152" s="14"/>
+      <c r="E152" s="5"/>
+      <c r="F152" s="5"/>
+      <c r="G152" s="5"/>
+      <c r="H152" s="5"/>
+      <c r="I152" s="5"/>
+      <c r="J152" s="5"/>
+      <c r="K152" s="5"/>
     </row>
     <row r="153" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="9"/>
+      <c r="A153" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="B153" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C153" s="24"/>
+        <v>98</v>
+      </c>
+      <c r="C153" s="24">
+        <v>18</v>
+      </c>
       <c r="D153" s="14"/>
       <c r="E153" s="5"/>
       <c r="F153" s="5"/>
@@ -4116,9 +4221,15 @@
       <c r="K153" s="5"/>
     </row>
     <row r="154" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A154" s="9"/>
-      <c r="B154" s="9"/>
-      <c r="C154" s="24"/>
+      <c r="A154" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B154" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C154" s="24">
+        <v>18</v>
+      </c>
       <c r="D154" s="14"/>
       <c r="E154" s="5"/>
       <c r="F154" s="5"/>
@@ -4129,9 +4240,15 @@
       <c r="K154" s="5"/>
     </row>
     <row r="155" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="9"/>
-      <c r="B155" s="9"/>
-      <c r="C155" s="24"/>
+      <c r="A155" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C155" s="24">
+        <v>18</v>
+      </c>
       <c r="D155" s="14"/>
       <c r="E155" s="5"/>
       <c r="F155" s="5"/>
@@ -4193,23 +4310,33 @@
       <c r="J159" s="5"/>
       <c r="K159" s="5"/>
     </row>
-    <row r="160" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="9"/>
-      <c r="B160" s="9"/>
-      <c r="C160" s="24"/>
-      <c r="D160" s="14"/>
-      <c r="E160" s="5"/>
-      <c r="F160" s="5"/>
-      <c r="G160" s="5"/>
-      <c r="H160" s="5"/>
-      <c r="I160" s="5"/>
-      <c r="J160" s="5"/>
-      <c r="K160" s="5"/>
+    <row r="160" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A160" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C160" s="21"/>
+      <c r="D160" s="12"/>
+      <c r="E160" s="10"/>
+      <c r="F160" s="10"/>
+      <c r="G160" s="10"/>
+      <c r="H160" s="10"/>
+      <c r="I160" s="10"/>
+      <c r="J160" s="10"/>
+      <c r="K160" s="10"/>
     </row>
     <row r="161" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A161" s="9"/>
-      <c r="B161" s="9"/>
-      <c r="C161" s="24"/>
+      <c r="A161" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C161" s="24">
+        <v>24</v>
+      </c>
       <c r="D161" s="14"/>
       <c r="E161" s="5"/>
       <c r="F161" s="5"/>
@@ -4219,29 +4346,35 @@
       <c r="J161" s="5"/>
       <c r="K161" s="5"/>
     </row>
-    <row r="162" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A162" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B162" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C162" s="21"/>
-      <c r="D162" s="12"/>
-      <c r="E162" s="10"/>
-      <c r="F162" s="10"/>
-      <c r="G162" s="10"/>
-      <c r="H162" s="10"/>
-      <c r="I162" s="10"/>
-      <c r="J162" s="10"/>
-      <c r="K162" s="10"/>
+    <row r="162" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A162" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C162" s="24">
+        <v>24</v>
+      </c>
+      <c r="D162" s="14"/>
+      <c r="E162" s="5"/>
+      <c r="F162" s="5"/>
+      <c r="G162" s="5"/>
+      <c r="H162" s="5"/>
+      <c r="I162" s="5"/>
+      <c r="J162" s="5"/>
+      <c r="K162" s="5"/>
     </row>
     <row r="163" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="9"/>
+      <c r="A163" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="B163" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C163" s="24"/>
+        <v>104</v>
+      </c>
+      <c r="C163" s="24">
+        <v>30</v>
+      </c>
       <c r="D163" s="14"/>
       <c r="E163" s="5"/>
       <c r="F163" s="5"/>
@@ -4329,22 +4462,28 @@
       <c r="J169" s="5"/>
       <c r="K169" s="5"/>
     </row>
-    <row r="170" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A170" s="9"/>
-      <c r="B170" s="9"/>
-      <c r="C170" s="24"/>
-      <c r="D170" s="14"/>
-      <c r="E170" s="5"/>
-      <c r="F170" s="5"/>
-      <c r="G170" s="5"/>
-      <c r="H170" s="5"/>
-      <c r="I170" s="5"/>
-      <c r="J170" s="5"/>
-      <c r="K170" s="5"/>
+    <row r="170" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A170" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C170" s="21"/>
+      <c r="D170" s="12"/>
+      <c r="E170" s="10"/>
+      <c r="F170" s="10"/>
+      <c r="G170" s="10"/>
+      <c r="H170" s="10"/>
+      <c r="I170" s="10"/>
+      <c r="J170" s="10"/>
+      <c r="K170" s="10"/>
     </row>
     <row r="171" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="9"/>
-      <c r="B171" s="9"/>
+      <c r="B171" s="9" t="s">
+        <v>106</v>
+      </c>
       <c r="C171" s="24"/>
       <c r="D171" s="14"/>
       <c r="E171" s="5"/>
@@ -4355,28 +4494,22 @@
       <c r="J171" s="5"/>
       <c r="K171" s="5"/>
     </row>
-    <row r="172" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A172" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B172" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C172" s="21"/>
-      <c r="D172" s="12"/>
-      <c r="E172" s="10"/>
-      <c r="F172" s="10"/>
-      <c r="G172" s="10"/>
-      <c r="H172" s="10"/>
-      <c r="I172" s="10"/>
-      <c r="J172" s="10"/>
-      <c r="K172" s="10"/>
+    <row r="172" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A172" s="9"/>
+      <c r="B172" s="9"/>
+      <c r="C172" s="24"/>
+      <c r="D172" s="14"/>
+      <c r="E172" s="5"/>
+      <c r="F172" s="5"/>
+      <c r="G172" s="5"/>
+      <c r="H172" s="5"/>
+      <c r="I172" s="5"/>
+      <c r="J172" s="5"/>
+      <c r="K172" s="5"/>
     </row>
     <row r="173" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="9"/>
-      <c r="B173" s="9" t="s">
-        <v>111</v>
-      </c>
+      <c r="B173" s="9"/>
       <c r="C173" s="24"/>
       <c r="D173" s="14"/>
       <c r="E173" s="5"/>
@@ -4426,31 +4559,23 @@
       <c r="J176" s="5"/>
       <c r="K176" s="5"/>
     </row>
-    <row r="177" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A177" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B177" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C177" s="21"/>
-      <c r="D177" s="12"/>
-      <c r="E177" s="10"/>
-      <c r="F177" s="10"/>
-      <c r="G177" s="10"/>
-      <c r="H177" s="10"/>
-      <c r="I177" s="10"/>
-      <c r="J177" s="10"/>
-      <c r="K177" s="10"/>
+    <row r="177" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A177" s="9"/>
+      <c r="B177" s="9"/>
+      <c r="C177" s="24"/>
+      <c r="D177" s="14"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="5"/>
+      <c r="G177" s="5"/>
+      <c r="H177" s="5"/>
+      <c r="I177" s="5"/>
+      <c r="J177" s="5"/>
+      <c r="K177" s="5"/>
     </row>
     <row r="178" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="9"/>
-      <c r="B178" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C178" s="24">
-        <v>16</v>
-      </c>
+      <c r="B178" s="9"/>
+      <c r="C178" s="24"/>
       <c r="D178" s="14"/>
       <c r="E178" s="5"/>
       <c r="F178" s="5"/>
@@ -4462,12 +4587,8 @@
     </row>
     <row r="179" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="9"/>
-      <c r="B179" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C179" s="24">
-        <v>16</v>
-      </c>
+      <c r="B179" s="9"/>
+      <c r="C179" s="24"/>
       <c r="D179" s="14"/>
       <c r="E179" s="5"/>
       <c r="F179" s="5"/>
@@ -4477,26 +4598,28 @@
       <c r="J179" s="5"/>
       <c r="K179" s="5"/>
     </row>
-    <row r="180" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A180" s="9"/>
-      <c r="B180" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C180" s="24">
-        <v>10</v>
-      </c>
-      <c r="D180" s="14"/>
-      <c r="E180" s="5"/>
-      <c r="F180" s="5"/>
-      <c r="G180" s="5"/>
-      <c r="H180" s="5"/>
-      <c r="I180" s="5"/>
-      <c r="J180" s="5"/>
-      <c r="K180" s="5"/>
+    <row r="180" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A180" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C180" s="21"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="10"/>
+      <c r="F180" s="10"/>
+      <c r="G180" s="10"/>
+      <c r="H180" s="10"/>
+      <c r="I180" s="10"/>
+      <c r="J180" s="10"/>
+      <c r="K180" s="10"/>
     </row>
     <row r="181" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181" s="9"/>
-      <c r="B181" s="9"/>
+      <c r="B181" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="C181" s="24"/>
       <c r="D181" s="14"/>
       <c r="E181" s="5"/>
@@ -4546,33 +4669,23 @@
       <c r="J184" s="5"/>
       <c r="K184" s="5"/>
     </row>
-    <row r="185" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A185" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B185" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C185" s="21"/>
-      <c r="D185" s="12"/>
-      <c r="E185" s="10"/>
-      <c r="F185" s="10"/>
-      <c r="G185" s="10"/>
-      <c r="H185" s="10"/>
-      <c r="I185" s="10"/>
-      <c r="J185" s="10"/>
-      <c r="K185" s="10"/>
+    <row r="185" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A185" s="9"/>
+      <c r="B185" s="9"/>
+      <c r="C185" s="24"/>
+      <c r="D185" s="14"/>
+      <c r="E185" s="5"/>
+      <c r="F185" s="5"/>
+      <c r="G185" s="5"/>
+      <c r="H185" s="5"/>
+      <c r="I185" s="5"/>
+      <c r="J185" s="5"/>
+      <c r="K185" s="5"/>
     </row>
     <row r="186" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B186" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C186" s="24">
-        <v>12</v>
-      </c>
+      <c r="A186" s="9"/>
+      <c r="B186" s="9"/>
+      <c r="C186" s="24"/>
       <c r="D186" s="14"/>
       <c r="E186" s="5"/>
       <c r="F186" s="5"/>
@@ -4583,15 +4696,9 @@
       <c r="K186" s="5"/>
     </row>
     <row r="187" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A187" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B187" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C187" s="24">
-        <v>12</v>
-      </c>
+      <c r="A187" s="9"/>
+      <c r="B187" s="9"/>
+      <c r="C187" s="24"/>
       <c r="D187" s="14"/>
       <c r="E187" s="5"/>
       <c r="F187" s="5"/>
@@ -4602,15 +4709,9 @@
       <c r="K187" s="5"/>
     </row>
     <row r="188" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A188" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B188" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C188" s="24">
-        <v>12</v>
-      </c>
+      <c r="A188" s="9"/>
+      <c r="B188" s="9"/>
+      <c r="C188" s="24"/>
       <c r="D188" s="14"/>
       <c r="E188" s="5"/>
       <c r="F188" s="5"/>
@@ -4621,15 +4722,9 @@
       <c r="K188" s="5"/>
     </row>
     <row r="189" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A189" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B189" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C189" s="24">
-        <v>12</v>
-      </c>
+      <c r="A189" s="9"/>
+      <c r="B189" s="9"/>
+      <c r="C189" s="24"/>
       <c r="D189" s="14"/>
       <c r="E189" s="5"/>
       <c r="F189" s="5"/>
@@ -4639,35 +4734,29 @@
       <c r="J189" s="5"/>
       <c r="K189" s="5"/>
     </row>
-    <row r="190" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A190" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B190" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C190" s="24">
-        <v>12</v>
-      </c>
-      <c r="D190" s="14"/>
-      <c r="E190" s="5"/>
-      <c r="F190" s="5"/>
-      <c r="G190" s="5"/>
-      <c r="H190" s="5"/>
-      <c r="I190" s="5"/>
-      <c r="J190" s="5"/>
-      <c r="K190" s="5"/>
+    <row r="190" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A190" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C190" s="21"/>
+      <c r="D190" s="12"/>
+      <c r="E190" s="10"/>
+      <c r="F190" s="10"/>
+      <c r="G190" s="10"/>
+      <c r="H190" s="10"/>
+      <c r="I190" s="10"/>
+      <c r="J190" s="10"/>
+      <c r="K190" s="10"/>
     </row>
     <row r="191" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A191" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="A191" s="9"/>
       <c r="B191" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C191" s="24">
-        <v>12</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C191" s="24"/>
       <c r="D191" s="14"/>
       <c r="E191" s="5"/>
       <c r="F191" s="5"/>
@@ -4678,15 +4767,9 @@
       <c r="K191" s="5"/>
     </row>
     <row r="192" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A192" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B192" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C192" s="24">
-        <v>12</v>
-      </c>
+      <c r="A192" s="9"/>
+      <c r="B192" s="9"/>
+      <c r="C192" s="24"/>
       <c r="D192" s="14"/>
       <c r="E192" s="5"/>
       <c r="F192" s="5"/>
@@ -4697,15 +4780,9 @@
       <c r="K192" s="5"/>
     </row>
     <row r="193" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A193" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B193" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C193" s="24">
-        <v>12</v>
-      </c>
+      <c r="A193" s="9"/>
+      <c r="B193" s="9"/>
+      <c r="C193" s="24"/>
       <c r="D193" s="14"/>
       <c r="E193" s="5"/>
       <c r="F193" s="5"/>
@@ -4728,12 +4805,31 @@
       <c r="J194" s="5"/>
       <c r="K194" s="5"/>
     </row>
-    <row r="196" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A195" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C195" s="21"/>
+      <c r="D195" s="12"/>
+      <c r="E195" s="10"/>
+      <c r="F195" s="10"/>
+      <c r="G195" s="10"/>
+      <c r="H195" s="10"/>
+      <c r="I195" s="10"/>
+      <c r="J195" s="10"/>
+      <c r="K195" s="10"/>
+    </row>
+    <row r="196" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A196" s="9"/>
-      <c r="B196" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C196" s="24"/>
+      <c r="B196" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C196" s="24">
+        <v>16</v>
+      </c>
       <c r="D196" s="14"/>
       <c r="E196" s="5"/>
       <c r="F196" s="5"/>
@@ -4746,10 +4842,10 @@
     <row r="197" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A197" s="9"/>
       <c r="B197" s="9" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="C197" s="24">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="D197" s="14"/>
       <c r="E197" s="5"/>
@@ -4763,10 +4859,10 @@
     <row r="198" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A198" s="9"/>
       <c r="B198" s="9" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
       <c r="C198" s="24">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D198" s="14"/>
       <c r="E198" s="5"/>
@@ -4779,12 +4875,8 @@
     </row>
     <row r="199" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A199" s="9"/>
-      <c r="B199" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C199" s="24">
-        <v>50</v>
-      </c>
+      <c r="B199" s="9"/>
+      <c r="C199" s="24"/>
       <c r="D199" s="14"/>
       <c r="E199" s="5"/>
       <c r="F199" s="5"/>
@@ -4796,12 +4888,8 @@
     </row>
     <row r="200" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A200" s="9"/>
-      <c r="B200" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C200" s="24">
-        <v>50</v>
-      </c>
+      <c r="B200" s="9"/>
+      <c r="C200" s="24"/>
       <c r="D200" s="14"/>
       <c r="E200" s="5"/>
       <c r="F200" s="5"/>
@@ -4813,12 +4901,8 @@
     </row>
     <row r="201" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="9"/>
-      <c r="B201" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C201" s="24">
-        <v>80</v>
-      </c>
+      <c r="B201" s="9"/>
+      <c r="C201" s="24"/>
       <c r="D201" s="14"/>
       <c r="E201" s="5"/>
       <c r="F201" s="5"/>
@@ -4830,12 +4914,8 @@
     </row>
     <row r="202" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A202" s="9"/>
-      <c r="B202" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C202" s="24">
-        <v>30</v>
-      </c>
+      <c r="B202" s="9"/>
+      <c r="C202" s="24"/>
       <c r="D202" s="14"/>
       <c r="E202" s="5"/>
       <c r="F202" s="5"/>
@@ -4845,30 +4925,32 @@
       <c r="J202" s="5"/>
       <c r="K202" s="5"/>
     </row>
-    <row r="203" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A203" s="9"/>
-      <c r="B203" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C203" s="24">
-        <v>100</v>
-      </c>
-      <c r="D203" s="14"/>
-      <c r="E203" s="5"/>
-      <c r="F203" s="5"/>
-      <c r="G203" s="5"/>
-      <c r="H203" s="5"/>
-      <c r="I203" s="5"/>
-      <c r="J203" s="5"/>
-      <c r="K203" s="5"/>
+    <row r="203" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A203" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C203" s="21"/>
+      <c r="D203" s="12"/>
+      <c r="E203" s="10"/>
+      <c r="F203" s="10"/>
+      <c r="G203" s="10"/>
+      <c r="H203" s="10"/>
+      <c r="I203" s="10"/>
+      <c r="J203" s="10"/>
+      <c r="K203" s="10"/>
     </row>
     <row r="204" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A204" s="9"/>
+      <c r="A204" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="B204" s="9" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="C204" s="24">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D204" s="14"/>
       <c r="E204" s="5"/>
@@ -4880,12 +4962,14 @@
       <c r="K204" s="5"/>
     </row>
     <row r="205" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A205" s="9"/>
+      <c r="A205" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="B205" s="9" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="C205" s="24">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="D205" s="14"/>
       <c r="E205" s="5"/>
@@ -4897,12 +4981,14 @@
       <c r="K205" s="5"/>
     </row>
     <row r="206" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A206" s="9"/>
+      <c r="A206" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="B206" s="9" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="C206" s="24">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D206" s="14"/>
       <c r="E206" s="5"/>
@@ -4914,9 +5000,15 @@
       <c r="K206" s="5"/>
     </row>
     <row r="207" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A207" s="9"/>
-      <c r="B207" s="9"/>
-      <c r="C207" s="24"/>
+      <c r="A207" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B207" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C207" s="24">
+        <v>12</v>
+      </c>
       <c r="D207" s="14"/>
       <c r="E207" s="5"/>
       <c r="F207" s="5"/>
@@ -4927,9 +5019,15 @@
       <c r="K207" s="5"/>
     </row>
     <row r="208" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A208" s="9"/>
-      <c r="B208" s="9"/>
-      <c r="C208" s="24"/>
+      <c r="A208" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B208" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C208" s="24">
+        <v>12</v>
+      </c>
       <c r="D208" s="14"/>
       <c r="E208" s="5"/>
       <c r="F208" s="5"/>
@@ -4940,9 +5038,15 @@
       <c r="K208" s="5"/>
     </row>
     <row r="209" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A209" s="9"/>
-      <c r="B209" s="9"/>
-      <c r="C209" s="24"/>
+      <c r="A209" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B209" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C209" s="24">
+        <v>12</v>
+      </c>
       <c r="D209" s="14"/>
       <c r="E209" s="5"/>
       <c r="F209" s="5"/>
@@ -4953,9 +5057,15 @@
       <c r="K209" s="5"/>
     </row>
     <row r="210" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A210" s="9"/>
-      <c r="B210" s="9"/>
-      <c r="C210" s="24"/>
+      <c r="A210" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B210" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C210" s="24">
+        <v>12</v>
+      </c>
       <c r="D210" s="14"/>
       <c r="E210" s="5"/>
       <c r="F210" s="5"/>
@@ -4965,17 +5075,289 @@
       <c r="J210" s="5"/>
       <c r="K210" s="5"/>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B211" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="C211" s="27">
-        <f>SUM(C2:C210)</f>
+    <row r="211" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A211" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B211" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C211" s="24">
+        <v>12</v>
+      </c>
+      <c r="D211" s="14"/>
+      <c r="E211" s="5"/>
+      <c r="F211" s="5"/>
+      <c r="G211" s="5"/>
+      <c r="H211" s="5"/>
+      <c r="I211" s="5"/>
+      <c r="J211" s="5"/>
+      <c r="K211" s="5"/>
+    </row>
+    <row r="212" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A212" s="9"/>
+      <c r="B212" s="9"/>
+      <c r="C212" s="24"/>
+      <c r="D212" s="14"/>
+      <c r="E212" s="5"/>
+      <c r="F212" s="5"/>
+      <c r="G212" s="5"/>
+      <c r="H212" s="5"/>
+      <c r="I212" s="5"/>
+      <c r="J212" s="5"/>
+      <c r="K212" s="5"/>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A213" s="53"/>
+    </row>
+    <row r="214" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A214" s="9"/>
+      <c r="B214" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C214" s="24"/>
+      <c r="D214" s="14"/>
+      <c r="E214" s="5"/>
+      <c r="F214" s="5"/>
+      <c r="G214" s="5"/>
+      <c r="H214" s="5"/>
+      <c r="I214" s="5"/>
+      <c r="J214" s="5"/>
+      <c r="K214" s="5"/>
+    </row>
+    <row r="215" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A215" s="9"/>
+      <c r="B215" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C215" s="24">
+        <v>40</v>
+      </c>
+      <c r="D215" s="14"/>
+      <c r="E215" s="5"/>
+      <c r="F215" s="5"/>
+      <c r="G215" s="5"/>
+      <c r="H215" s="5"/>
+      <c r="I215" s="5"/>
+      <c r="J215" s="5"/>
+      <c r="K215" s="5"/>
+    </row>
+    <row r="216" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A216" s="9"/>
+      <c r="B216" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C216" s="24">
+        <v>50</v>
+      </c>
+      <c r="D216" s="14"/>
+      <c r="E216" s="5"/>
+      <c r="F216" s="5"/>
+      <c r="G216" s="5"/>
+      <c r="H216" s="5"/>
+      <c r="I216" s="5"/>
+      <c r="J216" s="5"/>
+      <c r="K216" s="5"/>
+    </row>
+    <row r="217" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A217" s="9"/>
+      <c r="B217" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C217" s="24">
+        <v>50</v>
+      </c>
+      <c r="D217" s="14"/>
+      <c r="E217" s="5"/>
+      <c r="F217" s="5"/>
+      <c r="G217" s="5"/>
+      <c r="H217" s="5"/>
+      <c r="I217" s="5"/>
+      <c r="J217" s="5"/>
+      <c r="K217" s="5"/>
+    </row>
+    <row r="218" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A218" s="9"/>
+      <c r="B218" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C218" s="24">
+        <v>50</v>
+      </c>
+      <c r="D218" s="14"/>
+      <c r="E218" s="5"/>
+      <c r="F218" s="5"/>
+      <c r="G218" s="5"/>
+      <c r="H218" s="5"/>
+      <c r="I218" s="5"/>
+      <c r="J218" s="5"/>
+      <c r="K218" s="5"/>
+    </row>
+    <row r="219" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A219" s="9"/>
+      <c r="B219" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C219" s="24">
+        <v>80</v>
+      </c>
+      <c r="D219" s="14"/>
+      <c r="E219" s="5"/>
+      <c r="F219" s="5"/>
+      <c r="G219" s="5"/>
+      <c r="H219" s="5"/>
+      <c r="I219" s="5"/>
+      <c r="J219" s="5"/>
+      <c r="K219" s="5"/>
+    </row>
+    <row r="220" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A220" s="9"/>
+      <c r="B220" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C220" s="24">
+        <v>30</v>
+      </c>
+      <c r="D220" s="14"/>
+      <c r="E220" s="5"/>
+      <c r="F220" s="5"/>
+      <c r="G220" s="5"/>
+      <c r="H220" s="5"/>
+      <c r="I220" s="5"/>
+      <c r="J220" s="5"/>
+      <c r="K220" s="5"/>
+    </row>
+    <row r="221" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A221" s="9"/>
+      <c r="B221" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C221" s="24">
+        <v>100</v>
+      </c>
+      <c r="D221" s="14"/>
+      <c r="E221" s="5"/>
+      <c r="F221" s="5"/>
+      <c r="G221" s="5"/>
+      <c r="H221" s="5"/>
+      <c r="I221" s="5"/>
+      <c r="J221" s="5"/>
+      <c r="K221" s="5"/>
+    </row>
+    <row r="222" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A222" s="9"/>
+      <c r="B222" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C222" s="24">
+        <v>20</v>
+      </c>
+      <c r="D222" s="14"/>
+      <c r="E222" s="5"/>
+      <c r="F222" s="5"/>
+      <c r="G222" s="5"/>
+      <c r="H222" s="5"/>
+      <c r="I222" s="5"/>
+      <c r="J222" s="5"/>
+      <c r="K222" s="5"/>
+    </row>
+    <row r="223" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A223" s="9"/>
+      <c r="B223" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C223" s="24">
+        <v>50</v>
+      </c>
+      <c r="D223" s="14"/>
+      <c r="E223" s="5"/>
+      <c r="F223" s="5"/>
+      <c r="G223" s="5"/>
+      <c r="H223" s="5"/>
+      <c r="I223" s="5"/>
+      <c r="J223" s="5"/>
+      <c r="K223" s="5"/>
+    </row>
+    <row r="224" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A224" s="9"/>
+      <c r="B224" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C224" s="24">
+        <v>40</v>
+      </c>
+      <c r="D224" s="14"/>
+      <c r="E224" s="5"/>
+      <c r="F224" s="5"/>
+      <c r="G224" s="5"/>
+      <c r="H224" s="5"/>
+      <c r="I224" s="5"/>
+      <c r="J224" s="5"/>
+      <c r="K224" s="5"/>
+    </row>
+    <row r="225" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A225" s="9"/>
+      <c r="B225" s="9"/>
+      <c r="C225" s="24"/>
+      <c r="D225" s="14"/>
+      <c r="E225" s="5"/>
+      <c r="F225" s="5"/>
+      <c r="G225" s="5"/>
+      <c r="H225" s="5"/>
+      <c r="I225" s="5"/>
+      <c r="J225" s="5"/>
+      <c r="K225" s="5"/>
+    </row>
+    <row r="226" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A226" s="9"/>
+      <c r="B226" s="9"/>
+      <c r="C226" s="24"/>
+      <c r="D226" s="14"/>
+      <c r="E226" s="5"/>
+      <c r="F226" s="5"/>
+      <c r="G226" s="5"/>
+      <c r="H226" s="5"/>
+      <c r="I226" s="5"/>
+      <c r="J226" s="5"/>
+      <c r="K226" s="5"/>
+    </row>
+    <row r="227" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A227" s="9"/>
+      <c r="B227" s="9"/>
+      <c r="C227" s="24"/>
+      <c r="D227" s="14"/>
+      <c r="E227" s="5"/>
+      <c r="F227" s="5"/>
+      <c r="G227" s="5"/>
+      <c r="H227" s="5"/>
+      <c r="I227" s="5"/>
+      <c r="J227" s="5"/>
+      <c r="K227" s="5"/>
+    </row>
+    <row r="228" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A228" s="9"/>
+      <c r="B228" s="9"/>
+      <c r="C228" s="24"/>
+      <c r="D228" s="14"/>
+      <c r="E228" s="5"/>
+      <c r="F228" s="5"/>
+      <c r="G228" s="5"/>
+      <c r="H228" s="5"/>
+      <c r="I228" s="5"/>
+      <c r="J228" s="5"/>
+      <c r="K228" s="5"/>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B229" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C229" s="27">
+        <f>SUM(C2:C228)</f>
         <v>1650</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D8:D45 D48:D55 D57:D69 D196:D200 D172:D184 D72:D95 D102:D110">
+  <conditionalFormatting sqref="D8:D45 D48:D55 D59:D72 D214:D218 D190:D202 D75:D103 D120:D128">
     <cfRule type="containsText" dxfId="47" priority="58" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D8)))</formula>
     </cfRule>
@@ -4986,103 +5368,103 @@
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D111:D120">
+  <conditionalFormatting sqref="D129:D138">
     <cfRule type="containsText" dxfId="44" priority="52" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D111)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D129)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="43" priority="53" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D111)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D129)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="42" priority="54" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D111)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D129)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D121:D131">
+  <conditionalFormatting sqref="D139:D149">
     <cfRule type="containsText" dxfId="41" priority="49" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D121)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D139)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="40" priority="50" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D121)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D139)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="39" priority="51" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D121)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D139)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D132:D141">
+  <conditionalFormatting sqref="D150:D159">
     <cfRule type="containsText" dxfId="38" priority="46" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D132)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D150)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="37" priority="47" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D132)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D150)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="36" priority="48" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D132)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D150)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D142:D151">
+  <conditionalFormatting sqref="D160:D169">
     <cfRule type="containsText" dxfId="35" priority="43" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D142)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D160)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D142)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D160)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D142)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D160)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D152:D161">
+  <conditionalFormatting sqref="D170:D179">
     <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D152)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D170)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D152)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D170)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D152)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D170)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D162:D171">
+  <conditionalFormatting sqref="D180:D189">
     <cfRule type="containsText" dxfId="29" priority="37" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D162)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D180)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="28" priority="38" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D162)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D180)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="27" priority="39" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D162)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D180)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D96:D101">
+  <conditionalFormatting sqref="D104:D119">
     <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D96)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D96)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D96)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D104)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D70:D71">
+  <conditionalFormatting sqref="D73:D74">
     <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D70)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D73)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D70)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D73)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D70)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D73)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D185:D194">
+  <conditionalFormatting sqref="D203:D212">
     <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D185)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D203)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D185)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D203)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D185)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D203)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46:D47">
@@ -5096,7 +5478,7 @@
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D46)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
+  <conditionalFormatting sqref="D56:D58">
     <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="NO COMENZADO">
       <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D56)))</formula>
     </cfRule>
@@ -5107,48 +5489,48 @@
       <formula>NOT(ISERROR(SEARCH("COMPLETADO",D56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D201">
+  <conditionalFormatting sqref="D219">
     <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D201)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D219)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D201)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D219)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D201)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D219)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D202">
+  <conditionalFormatting sqref="D220">
     <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D202)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D220)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D202)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D220)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D202)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D220)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D203">
+  <conditionalFormatting sqref="D221">
     <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D203)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D221)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D203)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D221)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D203)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D221)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D204:D210">
+  <conditionalFormatting sqref="D222:D228">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO COMENZADO">
-      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D204)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO COMENZADO",D222)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="EN PROGRESO">
-      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D204)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",D222)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="COMPLETADO">
-      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D204)))</formula>
+      <formula>NOT(ISERROR(SEARCH("COMPLETADO",D222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>